<commit_message>
Add US related to Linguistics domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Chain-of-Thought dataset/CoTDataset.xlsx
+++ b/refair-server/datasets/Chain-of-Thought dataset/CoTDataset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Dataset ReFair\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\Chain-of-Thought dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEF8E74-EC2A-4AF1-AA78-7EA09C48CA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AE4D87-FD9F-4D30-9888-143EC1A04B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="70">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -180,13 +180,79 @@
   </si>
   <si>
     <t>As a library data analyst, I need to employ word embedding techniques to analyze book reviews and reader feedback, extracting key themes and sentiments to understand patron preferences and improve collection curation.</t>
+  </si>
+  <si>
+    <t>Linguistics</t>
+  </si>
+  <si>
+    <t>ReAdjusted_CoTPrompt</t>
+  </si>
+  <si>
+    <t>As a linguist, I want to apply adversarial learning techniques to detect and mitigate biases in language models, so that I can ensure fair representation across different dialects and linguistic variations.</t>
+  </si>
+  <si>
+    <t>As a researcher in historical linguistics, I want to apply CNNs to analyze patterns in ancient manuscripts and inscriptions, helping me understand the evolution of written languages over centuries.</t>
+  </si>
+  <si>
+    <t>As a researcher in computational linguistics, I want to create a conversational agent capable of simulating historical dialogues in ancient languages, enabling scholars to interact and explore linguistic contexts of past civilizations.</t>
+  </si>
+  <si>
+    <t>As a historical linguist, I want to apply decision tree models to classify and date linguistic artifacts based on stylistic and lexical features, facilitating the study of language evolution over centuries.</t>
+  </si>
+  <si>
+    <t>As a computational philologist, I want to create a document classification system using machine learning to categorize ancient manuscripts into different linguistic families or language groups, aiding in the study of historical linguistics and language evolution.</t>
+  </si>
+  <si>
+    <t>As a computational ethnolinguist, I want to build an entity extraction tool to automatically detect and classify cultural terms and expressions from ethnographic texts, aiding in the preservation and documentation of endangered languages and cultures.</t>
+  </si>
+  <si>
+    <t>As a computational sociolinguist, I want to address class imbalance in language variation datasets when studying rare linguistic phenomena, ensuring that minority dialects or less common linguistic features are adequately represented in statistical analyses.</t>
+  </si>
+  <si>
+    <t>As a computational sociolinguist, I want to use feature selection algorithms to identify the linguistic variables that best explain regional dialectal differences in speech patterns, helping me analyze sociolinguistic phenomena across diverse communities.</t>
+  </si>
+  <si>
+    <t>As a researcher in historical linguistics, I want to use keyword extraction algorithms to identify significant lexical changes in historical manuscripts, helping me track linguistic shifts and borrowings over different periods.</t>
+  </si>
+  <si>
+    <t>As a computational linguist, I want to apply k-Nearest Neighbor algorithm to classify phonetic features extracted from speech data, enabling me to study regional accents and phonological variations across different dialects.</t>
+  </si>
+  <si>
+    <t>As a computational stylistician, I want to apply multi-label classification to classify literary texts into multiple genres (e.g., drama, poetry, prose) based on stylistic features, aiding in literary analysis and genre classification studies.</t>
+  </si>
+  <si>
+    <t>As a phonetics researcher, I want to use a neural network model to classify speech sounds into phonetic categories, helping me analyze acoustic patterns and phonological variations across different languages.</t>
+  </si>
+  <si>
+    <t>As a computational lexicographer, I want to build a random forest classifier to categorize words into different semantic categories (e.g., nouns, verbs, adjectives) based on lexical and syntactic features, aiding in the development of comprehensive lexical databases.</t>
+  </si>
+  <si>
+    <t>As a computational linguist, I want to develop a semantic similarity model using machine learning techniques to measure the similarity between words and phrases across different languages, aiding in cross-linguistic semantic analysis and translation tasks.</t>
+  </si>
+  <si>
+    <t>As a linguistic data scientist, I want to implement sentiment analysis algorithms to analyze sentiment shifts in historical texts over time, helping me study evolving attitudes and cultural changes reflected in language use.</t>
+  </si>
+  <si>
+    <t>As a computational dialectologist, I want to create a speech-to-text model specialized in transcribing regional dialects and accents, enabling me to analyze linguistic variation and geographical distribution of dialectal features.</t>
+  </si>
+  <si>
+    <t>As a computational linguist, I want to develop a text categorization system to classify texts into different linguistic genres (e.g., narrative, expository, argumentative) based on textual features, aiding in genre analysis and linguistic research.</t>
+  </si>
+  <si>
+    <t>As a computational sociolinguist, I want to apply unsupervised clustering algorithms to identify distinct speech communities within a region based on linguistic features, helping me analyze language variation and dialectal boundaries.</t>
+  </si>
+  <si>
+    <t>As a computational sociolinguist, I want to build a voice recognition model capable of recognizing and categorizing regional accents and sociolectal variations in spoken language, aiding in sociolinguistic research on language variation.</t>
+  </si>
+  <si>
+    <t>As a researcher in historical linguistics, I want to apply word embedding models to track lexical changes and semantic evolution of words across different historical periods and languages, aiding in the study of language diachrony.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +278,19 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -240,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -248,6 +327,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -582,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="D25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -633,6 +714,9 @@
       <c r="E2" t="s">
         <v>28</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -650,6 +734,9 @@
       <c r="E3" t="s">
         <v>29</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -667,6 +754,9 @@
       <c r="E4" t="s">
         <v>30</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -684,6 +774,9 @@
       <c r="E5" t="s">
         <v>31</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -701,6 +794,9 @@
       <c r="E6" t="s">
         <v>32</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -718,6 +814,9 @@
       <c r="E7" t="s">
         <v>33</v>
       </c>
+      <c r="F7" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -735,6 +834,9 @@
       <c r="E8" t="s">
         <v>34</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
@@ -752,6 +854,9 @@
       <c r="E9" t="s">
         <v>36</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -769,6 +874,9 @@
       <c r="E10" t="s">
         <v>35</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -786,6 +894,9 @@
       <c r="E11" t="s">
         <v>37</v>
       </c>
+      <c r="F11" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -803,6 +914,9 @@
       <c r="E12" t="s">
         <v>38</v>
       </c>
+      <c r="F12" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -820,6 +934,9 @@
       <c r="E13" t="s">
         <v>39</v>
       </c>
+      <c r="F13" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -837,6 +954,9 @@
       <c r="E14" t="s">
         <v>41</v>
       </c>
+      <c r="F14" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -854,6 +974,9 @@
       <c r="E15" t="s">
         <v>40</v>
       </c>
+      <c r="F15" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
@@ -871,8 +994,11 @@
       <c r="E16" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="F16" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
@@ -888,8 +1014,11 @@
       <c r="E17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="F17" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
@@ -905,8 +1034,11 @@
       <c r="E18" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="F18" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
@@ -922,8 +1054,11 @@
       <c r="E19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="F19" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>4</v>
       </c>
@@ -939,8 +1074,11 @@
       <c r="E20" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="F20" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>4</v>
       </c>
@@ -955,6 +1093,349 @@
       </c>
       <c r="E21" t="s">
         <v>47</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="5">
+        <v>5</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="5">
+        <v>5</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="5">
+        <v>5</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="5">
+        <v>5</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="5">
+        <v>5</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="5">
+        <v>5</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="5">
+        <v>5</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="5">
+        <v>5</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="5">
+        <v>5</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="5">
+        <v>5</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="5">
+        <v>5</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="5">
+        <v>5</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="5">
+        <v>5</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="5">
+        <v>5</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="5">
+        <v>5</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="5">
+        <v>5</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="5">
+        <v>5</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="5">
+        <v>5</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="5">
+        <v>5</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="5">
+        <v>5</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add US related to Literature domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Chain-of-Thought dataset/CoTDataset.xlsx
+++ b/refair-server/datasets/Chain-of-Thought dataset/CoTDataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\Chain-of-Thought dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AE4D87-FD9F-4D30-9888-143EC1A04B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D362B36E-1262-4D2C-99DB-61B7019DBA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="91">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -246,13 +246,76 @@
   </si>
   <si>
     <t>As a researcher in historical linguistics, I want to apply word embedding models to track lexical changes and semantic evolution of words across different historical periods and languages, aiding in the study of language diachrony.</t>
+  </si>
+  <si>
+    <t>Literature</t>
+  </si>
+  <si>
+    <t>As a curator of digital literary archives, I propose using adversarial learning frameworks to detect and combat the spread of misinformation and fake news related to literary figures and historical contexts, preserving the authenticity of literary information online.</t>
+  </si>
+  <si>
+    <t>As a curator of digital literary collections, I plan to employ CNN techniques to automatically extract and summarize critical reviews and analyses of literary works from scholarly journals and publications, creating comprehensive meta-reviews for researchers and enthusiasts.</t>
+  </si>
+  <si>
+    <t>As a literature enthusiast, I want to interact with a conversational agent that uses natural language processing to discuss and recommend books based on my reading preferences and previous literary interests.</t>
+  </si>
+  <si>
+    <t>As a literary scholar, I aim to utilize decision tree algorithms to analyze the narrative structures and plot developments of classic novels, providing insights into the evolution of storytelling techniques over different literary epochs.</t>
+  </si>
+  <si>
+    <t>As a literary researcher, I want to develop a document classification system using machine learning to automatically categorize literary works by genre, enabling more efficient and accurate organization of digital literary archives.</t>
+  </si>
+  <si>
+    <t>As a researcher in comparative literature, I need an entity extraction tool to identify and compare the use of specific cultural and mythological references across different literary traditions, providing insights into cross-cultural influences and adaptations.</t>
+  </si>
+  <si>
+    <t>As a researcher in narrative studies, I want to use feature selection algorithms to extract key narrative elements (such as plot twists, character development) from literary works, enabling detailed comparative analysis across different storytelling traditions.</t>
+  </si>
+  <si>
+    <t>As a digital archivist, I aim to develop classification models that can handle imbalanced datasets to accurately categorize both popular and obscure literary texts, ensuring comprehensive digital collections that reflect literary diversity.</t>
+  </si>
+  <si>
+    <t>As a literary researcher, I want to use keyword extraction techniques to automatically identify and highlight key themes and motifs in large corpora of literary texts, facilitating thematic analysis and comparative studies.</t>
+  </si>
+  <si>
+    <t>As a literary analyst, I need to implement a k-nearest neighbor algorithm to classify literary texts based on stylistic features such as sentence length, vocabulary richness, and syntactic complexity, enabling comparative analysis across different authors and periods.</t>
+  </si>
+  <si>
+    <t>As a digital curator of literary collections, I aim to implement multi-label classification algorithms to categorize literary works into multiple genres or subgenres, providing users with more detailed and granular access to diverse literary categories in digital libraries.</t>
+  </si>
+  <si>
+    <t>As a literary researcher, I need to develop a random forest model to classify literary texts into different genres based on a combination of textual features such as vocabulary usage, sentence structure, and thematic elements, facilitating comprehensive genre analysis.</t>
+  </si>
+  <si>
+    <t>As a literary analyst, I want to develop a neural network model to identify and classify thematic elements in literary texts, enabling a deeper understanding of recurring motifs and their variations across different authors and periods.</t>
+  </si>
+  <si>
+    <t>As a curator of literary anthologies, I want to use semantic similarity techniques to group poems and short stories by thematic and stylistic affinities, creating more cohesive and engaging collections for readers.</t>
+  </si>
+  <si>
+    <t>As a literary archivist, I aim to develop a speech to text system to transcribe oral history interviews with authors and literary figures, preserving their narratives and insights for future literary research and biographical studies.</t>
+  </si>
+  <si>
+    <t>As a literary critic, I want to develop a sentiment analysis tool to assess the emotional resonance and public reception of contemporary poetry collections, helping to identify trends and preferences among readers.</t>
+  </si>
+  <si>
+    <t>As a researcher in comparative literature, I propose using text categorization algorithms to categorize novels from different cultures and languages into thematic groups, enabling cross-cultural analysis and understanding.</t>
+  </si>
+  <si>
+    <t>As a literary researcher, I propose using unsupervised clustering techniques to group poems and sonnets based on stylistic similarities and thematic motifs, enabling the discovery of hidden patterns and influences in poetic traditions.</t>
+  </si>
+  <si>
+    <t>As a literature educator, I propose using voice recognition technology in classrooms to assist students with disabilities in accessing and engaging with literary texts through spoken interactions and audio feedback.</t>
+  </si>
+  <si>
+    <t>As a literary researcher, I propose using word embedding techniques to analyze the semantic similarities between characters in novels from different literary periods, exploring recurring archetypes and motifs across diverse narratives.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,14 +341,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -327,8 +382,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -663,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -711,7 +766,7 @@
       <c r="D2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
         <v>28</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -719,40 +774,40 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
+        <v>17</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>49</v>
@@ -769,50 +824,50 @@
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
+        <v>25</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
+      <c r="A6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="3">
-        <v>5</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>5</v>
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>33</v>
+        <v>25</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>49</v>
@@ -829,50 +884,50 @@
         <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
+        <v>18</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3">
-        <v>5</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>5</v>
+      <c r="A9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="5">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>36</v>
+        <v>18</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="3">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>5</v>
+      <c r="A10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
+        <v>18</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>49</v>
@@ -889,50 +944,50 @@
         <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>37</v>
+        <v>9</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="3">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>5</v>
+      <c r="A12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="5">
+        <v>5</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" t="s">
-        <v>38</v>
+        <v>9</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3">
-        <v>5</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>5</v>
+      <c r="A13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="5">
+        <v>5</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>39</v>
+        <v>9</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>49</v>
@@ -949,50 +1004,50 @@
         <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" t="s">
-        <v>41</v>
+        <v>26</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="3">
-        <v>5</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>5</v>
+      <c r="A15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="5">
+        <v>5</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" t="s">
-        <v>40</v>
+        <v>26</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="3">
-        <v>5</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>5</v>
+      <c r="A16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="5">
+        <v>5</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" t="s">
-        <v>42</v>
+        <v>26</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>49</v>
@@ -1009,50 +1064,50 @@
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" t="s">
-        <v>44</v>
+        <v>20</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="3">
-        <v>5</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>5</v>
+      <c r="A18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="5">
+        <v>5</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" t="s">
-        <v>43</v>
+        <v>20</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="3">
-        <v>5</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="A19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="5">
+        <v>5</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" t="s">
-        <v>45</v>
+        <v>20</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>49</v>
@@ -1069,30 +1124,30 @@
         <v>5</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" t="s">
-        <v>46</v>
+        <v>22</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="3">
-        <v>5</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>5</v>
+      <c r="A21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="5">
+        <v>5</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" t="s">
-        <v>47</v>
+        <v>22</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>49</v>
@@ -1106,30 +1161,36 @@
         <v>5</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" t="s">
-        <v>50</v>
+        <v>22</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="5">
-        <v>5</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>48</v>
+      <c r="A23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" t="s">
-        <v>51</v>
+        <v>10</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
@@ -1143,10 +1204,13 @@
         <v>48</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
@@ -1157,30 +1221,36 @@
         <v>5</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" t="s">
-        <v>53</v>
+        <v>10</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="5">
-        <v>5</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>48</v>
+      <c r="A26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="3">
+        <v>5</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" t="s">
-        <v>54</v>
+        <v>21</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
@@ -1194,10 +1264,13 @@
         <v>48</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" t="s">
-        <v>55</v>
+        <v>21</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
@@ -1208,30 +1281,36 @@
         <v>5</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>57</v>
+        <v>79</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="5">
-        <v>5</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>48</v>
+      <c r="A29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="3">
+        <v>5</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" t="s">
-        <v>56</v>
+        <v>11</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
@@ -1245,10 +1324,13 @@
         <v>48</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" t="s">
-        <v>58</v>
+        <v>11</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
@@ -1259,33 +1341,39 @@
         <v>5</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E31" t="s">
-        <v>59</v>
+      <c r="E31" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="5">
-        <v>5</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>48</v>
+      <c r="A32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="3">
+        <v>5</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E32" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E32" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -1296,47 +1384,56 @@
         <v>48</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="5">
+        <v>5</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="3">
+        <v>5</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E33" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="5">
-        <v>5</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="5">
-        <v>5</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E35" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E35" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>4</v>
       </c>
@@ -1347,13 +1444,16 @@
         <v>48</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E36" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>4</v>
       </c>
@@ -1361,33 +1461,39 @@
         <v>5</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="5">
-        <v>5</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>48</v>
+        <v>12</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="3">
+        <v>5</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>4</v>
       </c>
@@ -1398,47 +1504,459 @@
         <v>48</v>
       </c>
       <c r="D39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="5">
+        <v>5</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="3">
+        <v>5</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="5">
+        <v>5</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="5">
+        <v>5</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="3">
+        <v>5</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="5">
+        <v>5</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="5">
+        <v>5</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="3">
+        <v>5</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="5">
+        <v>5</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="5">
+        <v>5</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="3">
+        <v>5</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="5">
+        <v>5</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="5">
+        <v>5</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="3">
+        <v>5</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E53" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="5">
+        <v>5</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="6" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" s="5">
-        <v>5</v>
-      </c>
-      <c r="C40" s="5" t="s">
+      <c r="F54" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="5">
+        <v>5</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="3">
+        <v>5</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" s="5">
+        <v>5</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E57" s="6" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="5">
-        <v>5</v>
-      </c>
-      <c r="C41" s="5" t="s">
+      <c r="F57" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" s="5">
+        <v>5</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="3">
+        <v>5</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="5">
+        <v>5</v>
+      </c>
+      <c r="C60" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="F60" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A61" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" s="5">
+        <v>5</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F61">
+    <sortCondition ref="D1:D61"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add US related to "Dermatology" and "Cardiology" domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Chain-of-Thought dataset/CoTDataset.xlsx
+++ b/refair-server/datasets/Chain-of-Thought dataset/CoTDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\Chain-of-Thought dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39DAC31-41B5-45FF-B026-2CC0A429D5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59414A9A-06CD-491F-AB21-FAE0BC936EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="262">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -693,6 +693,135 @@
   </si>
   <si>
     <t>As a trade economist, I want to employ word embedding models to analyze international trade agreements and policy documents, extracting key terms and understanding contextual relationships to assess economic impacts and support trade negotiations.</t>
+  </si>
+  <si>
+    <t>Medicine &amp; Health</t>
+  </si>
+  <si>
+    <t>Cardiology</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to utilize adversarial learning techniques to improve the robustness of my predictive models for heart disease risk assessment, ensuring that the models are resistant to adversarial attacks and provide reliable clinical insights.</t>
+  </si>
+  <si>
+    <t>Dermatology</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to leverage adversarial learning techniques to enhance the robustness of my skin condition classification models against potential adversarial attacks, ensuring reliable diagnoses and treatment recommendations.</t>
+  </si>
+  <si>
+    <t>As a researcher in cardiac imaging, I aim to develop CNN-based algorithms capable of detecting early signs of coronary artery disease from coronary CT angiography scans, enabling timely intervention and preventive care for patients at risk of heart attacks.</t>
+  </si>
+  <si>
+    <t>As a skincare researcher, I aim to develop CNN-based tools that can analyze facial photographs over time to track changes in skin conditions and assess the efficacy of skincare treatments, providing personalized recommendations for users.</t>
+  </si>
+  <si>
+    <t>As a patient, I want to interact with a conversational agent that uses machine learning to educate me about cardiovascular health, personalized risk factors, and lifestyle modifications, empowering me to make informed decisions for my well-being.</t>
+  </si>
+  <si>
+    <t>As a patient seeking dermatological advice, I want a conversational agent that uses machine learning to provide personalized skincare recommendations based on my skin type, concerns, and lifestyle habits, so that I can better manage and improve my skin health.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I want to use decision tree models to predict the likelihood of post-operative complications in cardiac surgery patients, based on pre-operative variables such as age, medical history, and surgical procedure type.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to use decision tree algorithms to classify skin lesions based on visual characteristics such as size, color, and texture, so that I can make accurate diagnoses and recommend appropriate treatments.</t>
+  </si>
+  <si>
+    <t>As a cardiac rehabilitation specialist, I want a document classification tool that can analyze patient feedback forms and session reports to categorize patient progress and adherence to rehabilitation programs, helping to tailor personalized treatment plans for optimal recovery outcomes.</t>
+  </si>
+  <si>
+    <t>As a healthcare administrator, I need a document classification model specialized in dermatology to organize patient records, lab reports, and medical notes according to different skin conditions, ensuring efficient retrieval of information for clinical decision-making and patient management.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I need an entity extraction model in machine learning to automatically extract key clinical parameters such as blood pressure readings, cholesterol levels, and heart rate variations from patient medical records, facilitating comprehensive cardiovascular risk assessments.</t>
+  </si>
+  <si>
+    <t>As a skincare researcher, I need an entity extraction model capable of parsing clinical trial reports and extracting data on treatment efficacy metrics, adverse reactions, patient demographics, and treatment protocols for systematic analysis and comparison.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to implement feature selection techniques in machine learning to identify the most significant biomarkers and clinical variables from cardiac imaging data, enhancing the accuracy of diagnostic models for detecting coronary artery disease.</t>
+  </si>
+  <si>
+    <t>As a skincare researcher, I aim to use feature selection algorithms to analyze dermatological imaging data and identify key visual features (e.g., texture, color variation) associated with different types of skin lesions, aiding in automated diagnosis and treatment planning.</t>
+  </si>
+  <si>
+    <t>As a pharmaceutical researcher, I want to develop algorithms using imbalanced dataset methodologies to evaluate the efficacy and safety of new cardiovascular drugs in clinical trials, ensuring robust analysis of rare adverse reactions and treatment outcomes.</t>
+  </si>
+  <si>
+    <t>As a researcher studying dermatological adverse reactions, I aim to develop machine learning models that can effectively handle imbalanced datasets to predict the occurrence of rare but severe skin reactions to medications, facilitating early detection and prevention strategies.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to implement keyword extraction algorithms in machine learning to automatically identify and extract key terms related to cardiac health from medical research papers, enabling efficient literature review and staying updated with the latest advancements in cardiology.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to implement machine learning techniques for keyword extraction from patient medical histories and notes, to automatically identify and highlight key symptoms, treatments, and diagnostic indicators related to dermatological conditions, improving efficiency and accuracy in patient care.</t>
+  </si>
+  <si>
+    <t>As a cardiac rehabilitation specialist, I want to utilize k-Nearest Neighbor techniques to personalize exercise and rehabilitation plans for patients recovering from myocardial infarction, tailoring recommendations based on similarities to successful recovery cases.</t>
+  </si>
+  <si>
+    <t>As a skincare researcher, I aim to apply k-Nearest Neighbor methods to analyze patient skincare routines and product usage patterns, identifying similarities among individuals with similar skin types and conditions to personalize skincare recommendations.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to develop a multi-label classification model using machine learning to predict the presence of multiple cardiac conditions (e.g., hypertension, atrial fibrillation, coronary artery disease) from patient data, enabling comprehensive risk assessment and personalized treatment planning.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to develop a multi-label classification model using machine learning to categorize skin conditions based on symptoms such as rash, itchiness, and discoloration, allowing for comprehensive diagnosis and treatment planning for patients with overlapping symptoms.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I aim to develop neural network models to predict patient outcomes following cardiac surgeries based on pre-operative risk factors, post-operative complications, and recovery progress, enhancing prognostic accuracy and patient care management.</t>
+  </si>
+  <si>
+    <t>As a skincare researcher, I aim to train a neural network for predictive modeling of skincare product effectiveness based on ingredients and user skin type data, allowing for personalized recommendations and improved consumer satisfaction.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to utilize a random forest algorithm to analyze patient data including age, lifestyle factors, and medical history to predict the likelihood of developing cardiovascular diseases such as coronary artery disease and heart failure, aiding in early intervention and preventive care.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to develop a random forest model to predict the likelihood of developing skin allergies based on patient demographics, environmental factors, and genetic predispositions, allowing for early preventive measures and personalized patient care.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to develop a semantic similarity model in natural language processing to compare and categorize clinical notes and patient reports based on their relevance to specific cardiac conditions and symptoms, aiding in efficient information retrieval and decision-making.</t>
+  </si>
+  <si>
+    <t>As a skincare product developer, I aim to use NLP techniques for semantic similarity to analyze customer reviews and feedback on skincare products, identifying common concerns and preferences among users to inform product improvement strategies.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I want to apply sentiment analysis to patient feedback collected from cardiac rehabilitation programs, to understand patient satisfaction levels and identify areas for improvement in our services.</t>
+  </si>
+  <si>
+    <t>As a skincare product developer, I need to perform sentiment analysis on customer reviews and social media comments about our products to understand customer satisfaction levels and identify areas for product improvement in the skincare industry.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to implement speech-to-text technology in clinical settings to transcribe patient interviews and discussions accurately, facilitating efficient documentation of symptoms, medical history, and treatment plans.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to use speech to text technology during patient consultations to automatically transcribe discussions about symptoms, medical history, and treatment preferences, improving accuracy and efficiency in clinical documentation.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I need a text categorization system to classify medical research articles into categories such as coronary artery disease, heart failure, and arrhythmias, facilitating quick access to relevant literature for evidence-based practice in cardiology.</t>
+  </si>
+  <si>
+    <t>As a skincare researcher, I want to implement text categorization algorithms to classify scientific articles and research papers in dermatology into topics such as skin cancer treatment, dermatological surgery techniques, and skincare product efficacy, facilitating literature review and research synthesis.</t>
+  </si>
+  <si>
+    <t>As a cardiovascular researcher, I want to apply unsupervised clustering algorithms to cardiac imaging data (e.g., MRI, CT scans) to identify distinct patterns of heart morphology and function, aiding in the classification of structural heart diseases and anomalies.</t>
+  </si>
+  <si>
+    <t>As a skincare product developer, I aim to use unsupervised clustering to analyze customer feedback and reviews on skincare products, identifying clusters of consumers with similar skin concerns and preferences to tailor product formulations and marketing strategies.</t>
+  </si>
+  <si>
+    <t>As a cardiac rehabilitation specialist, I aim to use voice recognition software for patients recovering from heart surgeries or cardiac events to record their daily progress and symptoms, facilitating remote monitoring and personalized care management.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I need a voice recognition system to transcribe patient consultations accurately, converting spoken descriptions of symptoms, medical history, and treatment preferences into text for efficient documentation and diagnosis.</t>
+  </si>
+  <si>
+    <t>As a medical researcher in cardiology, I want to develop word embedding models to analyze and categorize medical literature and research articles on specific cardiovascular topics such as heart failure management and coronary artery disease prevention, enabling efficient literature review and knowledge synthesis.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to use word embedding techniques to analyze patient medical records and identify key dermatological terms and concepts related to symptoms, treatments, and disease progression, enhancing information retrieval and clinical decision-making.</t>
   </si>
 </sst>
 </file>
@@ -736,9 +865,10 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -769,6 +899,12 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6D9EEB"/>
+        <bgColor rgb="FF6D9EEB"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -782,7 +918,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -798,6 +934,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1132,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F181"/>
+  <dimension ref="A1:F221"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A196" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C196" sqref="C196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4767,6 +4907,806 @@
         <v>49</v>
       </c>
     </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B182" s="11">
+        <v>6</v>
+      </c>
+      <c r="C182" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D182" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F182" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B183" s="11">
+        <v>6</v>
+      </c>
+      <c r="C183" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D183" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F183" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B184" s="11">
+        <v>6</v>
+      </c>
+      <c r="C184" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D184" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F184" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B185" s="11">
+        <v>6</v>
+      </c>
+      <c r="C185" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D185" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F185" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B186" s="11">
+        <v>6</v>
+      </c>
+      <c r="C186" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F186" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B187" s="11">
+        <v>6</v>
+      </c>
+      <c r="C187" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D187" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F187" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B188" s="11">
+        <v>6</v>
+      </c>
+      <c r="C188" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D188" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F188" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B189" s="11">
+        <v>6</v>
+      </c>
+      <c r="C189" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F189" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B190" s="11">
+        <v>6</v>
+      </c>
+      <c r="C190" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F190" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B191" s="11">
+        <v>6</v>
+      </c>
+      <c r="C191" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F191" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B192" s="11">
+        <v>6</v>
+      </c>
+      <c r="C192" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F192" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B193" s="11">
+        <v>6</v>
+      </c>
+      <c r="C193" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D193" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F193" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B194" s="11">
+        <v>6</v>
+      </c>
+      <c r="C194" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D194" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F194" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B195" s="11">
+        <v>6</v>
+      </c>
+      <c r="C195" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D195" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B196" s="11">
+        <v>6</v>
+      </c>
+      <c r="C196" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D196" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B197" s="11">
+        <v>6</v>
+      </c>
+      <c r="C197" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D197" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F197" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B198" s="11">
+        <v>6</v>
+      </c>
+      <c r="C198" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D198" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F198" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B199" s="11">
+        <v>6</v>
+      </c>
+      <c r="C199" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D199" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F199" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B200" s="11">
+        <v>6</v>
+      </c>
+      <c r="C200" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E200" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="F200" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B201" s="11">
+        <v>6</v>
+      </c>
+      <c r="C201" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D201" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F201" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B202" s="11">
+        <v>6</v>
+      </c>
+      <c r="C202" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D202" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B203" s="11">
+        <v>6</v>
+      </c>
+      <c r="C203" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D203" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F203" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B204" s="11">
+        <v>6</v>
+      </c>
+      <c r="C204" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D204" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F204" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B205" s="11">
+        <v>6</v>
+      </c>
+      <c r="C205" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D205" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F205" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B206" s="11">
+        <v>6</v>
+      </c>
+      <c r="C206" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D206" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F206" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B207" s="11">
+        <v>6</v>
+      </c>
+      <c r="C207" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D207" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F207" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B208" s="11">
+        <v>6</v>
+      </c>
+      <c r="C208" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D208" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F208" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B209" s="11">
+        <v>6</v>
+      </c>
+      <c r="C209" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D209" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F209" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B210" s="11">
+        <v>6</v>
+      </c>
+      <c r="C210" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D210" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F210" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B211" s="11">
+        <v>6</v>
+      </c>
+      <c r="C211" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F211" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B212" s="11">
+        <v>6</v>
+      </c>
+      <c r="C212" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D212" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F212" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B213" s="11">
+        <v>6</v>
+      </c>
+      <c r="C213" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D213" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F213" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B214" s="11">
+        <v>6</v>
+      </c>
+      <c r="C214" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D214" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F214" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A215" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B215" s="11">
+        <v>6</v>
+      </c>
+      <c r="C215" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D215" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F215" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B216" s="11">
+        <v>6</v>
+      </c>
+      <c r="C216" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D216" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F216" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B217" s="11">
+        <v>6</v>
+      </c>
+      <c r="C217" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D217" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F217" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A218" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B218" s="11">
+        <v>6</v>
+      </c>
+      <c r="C218" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D218" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F218" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B219" s="11">
+        <v>6</v>
+      </c>
+      <c r="C219" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D219" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F219" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B220" s="11">
+        <v>6</v>
+      </c>
+      <c r="C220" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D220" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F220" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B221" s="11">
+        <v>6</v>
+      </c>
+      <c r="C221" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D221" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F221" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A122:F181">
     <sortCondition ref="D1:D181"/>

</xml_diff>

<commit_message>
Add US related to "Endocrinology" and "Health" domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Chain-of-Thought dataset/CoTDataset.xlsx
+++ b/refair-server/datasets/Chain-of-Thought dataset/CoTDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\Chain-of-Thought dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59414A9A-06CD-491F-AB21-FAE0BC936EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFE0BA4-66D3-405D-B373-6E35A2F9ADDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="304">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -822,6 +822,132 @@
   </si>
   <si>
     <t>As a dermatologist, I want to use word embedding techniques to analyze patient medical records and identify key dermatological terms and concepts related to symptoms, treatments, and disease progression, enhancing information retrieval and clinical decision-making.</t>
+  </si>
+  <si>
+    <t>Endocrinology</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I need an adversarial learning model to enhance the robustness of hormone level predictions against noisy data inputs, ensuring more accurate diagnosis and treatment recommendations.</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to employ adversarial learning techniques to enhance the robustness of my deep learning models for medical image analysis, so that I can accurately detect subtle anomalies that traditional methods might miss.</t>
+  </si>
+  <si>
+    <t>As a researcher in endocrinology, I aim to develop a CNN model to analyze histopathological images of adrenal gland tissues, identifying structural abnormalities and patterns associated with adrenal tumors to assist pathologists in diagnosis.</t>
+  </si>
+  <si>
+    <t>As a public health researcher, I want to use CNNs to analyze satellite imagery and predict environmental factors influencing disease outbreaks, such as mosquito breeding grounds for vector-borne diseases, facilitating targeted preventive measures and interventions.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I need a conversational agent powered by machine learning to interact with patients, gather symptoms related to thyroid function, and recommend preliminary tests, assisting in early diagnosis and treatment.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I want a conversational agent powered by machine learning to assist patients in scheduling appointments and providing basic medical advice, so that our clinic can streamline patient management and improve accessibility to healthcare services.</t>
+  </si>
+  <si>
+    <t>As a researcher in endocrinology, I aim to develop a decision tree model using patient data to predict the risk of osteoporosis based on bone density measurements, hormone levels, and lifestyle factors, facilitating early intervention strategies.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I want to utilize a decision tree algorithm to classify patient symptoms and recommend appropriate diagnostic tests, so that we can achieve accurate and timely diagnoses for better patient management.</t>
+  </si>
+  <si>
+    <t>As a researcher in endocrinology, I want to develop a document classification model to classify patient electronic health records (EHRs) based on symptoms and diagnostic codes, enabling quick retrieval of relevant cases for retrospective studies and clinical research.</t>
+  </si>
+  <si>
+    <t>As a hospital administrator, I want to implement a document classification model to automatically categorize patient medical records based on their conditions (e.g., diabetes, hypertension) to streamline data retrieval and facilitate personalized patient care.</t>
+  </si>
+  <si>
+    <t>As a researcher in endocrinology, I need an entity extraction system to automatically identify and extract hormone names, levels, and trends from unstructured clinical notes and reports, enabling comprehensive analysis of patient hormonal profiles.</t>
+  </si>
+  <si>
+    <t>As a healthcare researcher, I want to develop an entity extraction system using machine learning to automatically identify and extract key medical terms (e.g., diseases, medications) from electronic health records, facilitating structured data analysis and clinical research.</t>
+  </si>
+  <si>
+    <t>As a researcher in endocrinology, I want to implement feature selection techniques to identify significant dietary factors influencing thyroid function in patients with autoimmune thyroid diseases, aiding in nutritional counseling and disease management.</t>
+  </si>
+  <si>
+    <t>As a healthcare data analyst, I want to use feature selection algorithms to streamline predictive modeling of patient readmission risks based on electronic health records, ensuring that only the most informative variables are included for accurate risk assessment.</t>
+  </si>
+  <si>
+    <t>As a researcher in endocrinology, I need to address class imbalance in datasets related to rare endocrine disorders (e.g., acromegaly, Cushing's syndrome) using techniques such as oversampling of minority classes or ensemble methods, to improve the accuracy of predictive models.</t>
+  </si>
+  <si>
+    <t>As a healthcare AI developer, I want to apply techniques for handling imbalanced datasets to develop a predictive model for early detection of adverse drug reactions, ensuring that rare but critical events are effectively captured and managed.</t>
+  </si>
+  <si>
+    <t>As a researcher in endocrinology, I want to develop a keyword extraction model to identify relevant keywords from patient health records pertaining to symptoms of hypothyroidism, aiding in efficient data retrieval and analysis for clinical studies.</t>
+  </si>
+  <si>
+    <t>As a healthcare IT specialist, I want to integrate keyword extraction algorithms into our electronic health record system to automatically extract and tag clinical concepts (e.g., symptoms, treatments) from unstructured patient notes, improving data interoperability and supporting clinical decision support systems.</t>
+  </si>
+  <si>
+    <t>As a researcher in endocrinology, I want to use KNN to classify patients into different risk groups for developing osteoporosis based on bone density measurements, hormonal levels, and lifestyle factors, to recommend personalized preventive measures.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to utilize k-NN algorithms to predict patient outcomes based on similar cases in historical patient data, enabling personalized treatment recommendations and improving overall healthcare outcomes.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I need a multi-label classification model to classify patient records into multiple endocrine disorders (e.g., diabetes, thyroid dysfunction, adrenal disorders) based on symptoms, laboratory tests, and genetic predispositions, to support accurate diagnosis and treatment.</t>
+  </si>
+  <si>
+    <t>As a public health analyst, I want to apply multi-label classification techniques to classify patient records based on multiple infectious diseases (e.g., tuberculosis, HIV) for surveillance and monitoring purposes, facilitating early detection and intervention in disease outbreaks.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I need a neural network-based system to classify thyroid ultrasound images into different categories (e.g., benign nodules, malignant nodules, cysts) based on texture features and structural characteristics, supporting accurate diagnosis and treatment planning.</t>
+  </si>
+  <si>
+    <t>As a healthcare IT developer, I want to implement a deep learning neural network to analyze real-time physiological data from wearable devices (e.g., heart rate, ECG) for early detection of cardiac abnormalities and timely alerting of healthcare providers and patients.</t>
+  </si>
+  <si>
+    <t>As a researcher in endocrinology, I want to develop a random forest algorithm to predict the risk of developing type 2 diabetes based on lifestyle factors (e.g., diet, exercise), genetic markers, and insulin resistance metrics, to guide early intervention and preventive measures.</t>
+  </si>
+  <si>
+    <t>As a healthcare data scientist, I want to develop a random forest model to predict patient outcomes following surgery based on a combination of pre-operative health metrics and surgical procedure details, enabling personalized post-operative care plans.</t>
+  </si>
+  <si>
+    <t>As a clinical researcher in endocrinology, I want to use semantic similarity models to explore relationships between medical literature and patient records, identifying novel treatments for rare hormonal disorders.</t>
+  </si>
+  <si>
+    <t>As a healthcare IT developer, I want to integrate semantic similarity models into a clinical decision support system to recommend relevant clinical guidelines and treatment protocols based on patient-specific symptoms and medical history.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I need sentiment analysis tools to analyze patient feedback from surveys about their experiences with hormone replacement therapies, allowing me to tailor treatments to meet patient expectations and improve adherence.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I want to implement sentiment analysis on patient feedback collected through surveys and social media to assess patient satisfaction levels with our healthcare services, enabling us to identify areas for improvement in patient care.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I need a speech to text system to transcribe patient consultations accurately, capturing details about symptoms and medical history to formulate precise treatment plans for hormone disorders.</t>
+  </si>
+  <si>
+    <t>As a healthcare IT specialist, I want to deploy speech-to-text algorithms to convert audio recordings of patient encounters into structured data for analysis and research purposes, enabling retrospective studies and clinical research advancements.</t>
+  </si>
+  <si>
+    <t>As a researcher in endocrinology, I want to develop a text categorization model to classify medical literature into different subfields such as thyroid disorders, diabetes management, and hormone replacement therapy, facilitating easier access to relevant research for specialists.</t>
+  </si>
+  <si>
+    <t>As a healthcare data analyst, I want to develop a text categorization system to classify medical research articles into specific categories (e.g., clinical trials, case studies) based on their content, facilitating easier literature review and research synthesis for medical professionals.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to use unsupervised clustering algorithms to analyze patient data and identify natural clusters of symptoms and biomarkers in diabetes patients, guiding personalized treatment plans and predictive modeling for disease progression.</t>
+  </si>
+  <si>
+    <t>As a healthcare IT specialist, I want to implement unsupervised clustering models to analyze patient demographics and health outcomes data to identify patterns of chronic disease prevalence and comorbidities, supporting population health management initiatives.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I need a voice recognition system to transcribe patient consultations accurately, capturing discussions on symptoms and treatment histories to enhance medical records for hormone-related conditions.</t>
+  </si>
+  <si>
+    <t>As a healthcare researcher, I want to analyze voice recordings of patients with neurological conditions (e.g., Parkinson's disease, stroke) using voice recognition tools to identify subtle changes in speech patterns indicative of disease progression or treatment effectiveness.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I aim to apply word embedding models to analyze patient records and identify patterns in hormone profiles associated with metabolic syndrome, aiding in early detection and personalized treatment strategies.</t>
+  </si>
+  <si>
+    <t>As a biomedical researcher, I want to apply word embedding techniques to analyze electronic health records and identify semantic relationships between medical terms (e.g., symptoms, treatments), facilitating more accurate automated diagnosis and treatment recommendation systems.</t>
   </si>
 </sst>
 </file>
@@ -1272,10 +1398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F221"/>
+  <dimension ref="A1:F261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C196" sqref="C196"/>
+    <sheetView tabSelected="1" topLeftCell="E236" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F221" sqref="F221:F261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4955,13 +5081,13 @@
         <v>6</v>
       </c>
       <c r="C184" s="11" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>224</v>
+        <v>263</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>49</v>
@@ -4975,13 +5101,13 @@
         <v>6</v>
       </c>
       <c r="C185" s="11" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="F185" s="1" t="s">
         <v>49</v>
@@ -4998,10 +5124,10 @@
         <v>220</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>49</v>
@@ -5018,10 +5144,10 @@
         <v>222</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>49</v>
@@ -5035,13 +5161,13 @@
         <v>6</v>
       </c>
       <c r="C188" s="11" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>228</v>
+        <v>266</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>49</v>
@@ -5055,13 +5181,13 @@
         <v>6</v>
       </c>
       <c r="C189" s="11" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>229</v>
+        <v>267</v>
       </c>
       <c r="F189" s="1" t="s">
         <v>49</v>
@@ -5078,10 +5204,10 @@
         <v>220</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>49</v>
@@ -5098,10 +5224,10 @@
         <v>222</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="F191" s="1" t="s">
         <v>49</v>
@@ -5115,13 +5241,13 @@
         <v>6</v>
       </c>
       <c r="C192" s="11" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="F192" s="1" t="s">
         <v>49</v>
@@ -5135,13 +5261,13 @@
         <v>6</v>
       </c>
       <c r="C193" s="11" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>233</v>
+        <v>269</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>49</v>
@@ -5158,10 +5284,10 @@
         <v>220</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>49</v>
@@ -5178,10 +5304,10 @@
         <v>222</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="F195" s="1" t="s">
         <v>49</v>
@@ -5195,13 +5321,13 @@
         <v>6</v>
       </c>
       <c r="C196" s="11" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>236</v>
+        <v>270</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>49</v>
@@ -5215,13 +5341,13 @@
         <v>6</v>
       </c>
       <c r="C197" s="11" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>237</v>
+        <v>271</v>
       </c>
       <c r="F197" s="1" t="s">
         <v>49</v>
@@ -5238,10 +5364,10 @@
         <v>220</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>49</v>
@@ -5258,10 +5384,10 @@
         <v>222</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>49</v>
@@ -5275,13 +5401,13 @@
         <v>6</v>
       </c>
       <c r="C200" s="11" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E200" s="12" t="s">
-        <v>240</v>
+        <v>26</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>49</v>
@@ -5295,13 +5421,13 @@
         <v>6</v>
       </c>
       <c r="C201" s="11" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>241</v>
+        <v>273</v>
       </c>
       <c r="F201" s="1" t="s">
         <v>49</v>
@@ -5318,10 +5444,10 @@
         <v>220</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>49</v>
@@ -5338,10 +5464,10 @@
         <v>222</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="F203" s="1" t="s">
         <v>49</v>
@@ -5355,13 +5481,13 @@
         <v>6</v>
       </c>
       <c r="C204" s="11" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>244</v>
+        <v>274</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>49</v>
@@ -5375,13 +5501,13 @@
         <v>6</v>
       </c>
       <c r="C205" s="11" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>245</v>
+        <v>275</v>
       </c>
       <c r="F205" s="1" t="s">
         <v>49</v>
@@ -5398,10 +5524,10 @@
         <v>220</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="F206" s="1" t="s">
         <v>49</v>
@@ -5418,10 +5544,10 @@
         <v>222</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="F207" s="1" t="s">
         <v>49</v>
@@ -5435,13 +5561,13 @@
         <v>6</v>
       </c>
       <c r="C208" s="11" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>248</v>
+        <v>276</v>
       </c>
       <c r="F208" s="1" t="s">
         <v>49</v>
@@ -5455,13 +5581,13 @@
         <v>6</v>
       </c>
       <c r="C209" s="11" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>249</v>
+        <v>277</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>49</v>
@@ -5478,10 +5604,10 @@
         <v>220</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="F210" s="1" t="s">
         <v>49</v>
@@ -5498,10 +5624,10 @@
         <v>222</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="F211" s="1" t="s">
         <v>49</v>
@@ -5515,13 +5641,13 @@
         <v>6</v>
       </c>
       <c r="C212" s="11" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
       <c r="F212" s="1" t="s">
         <v>49</v>
@@ -5535,13 +5661,13 @@
         <v>6</v>
       </c>
       <c r="C213" s="11" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>253</v>
+        <v>279</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>49</v>
@@ -5558,10 +5684,10 @@
         <v>220</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="F214" s="1" t="s">
         <v>49</v>
@@ -5578,10 +5704,10 @@
         <v>222</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="F215" s="1" t="s">
         <v>49</v>
@@ -5595,13 +5721,13 @@
         <v>6</v>
       </c>
       <c r="C216" s="11" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>256</v>
+        <v>280</v>
       </c>
       <c r="F216" s="1" t="s">
         <v>49</v>
@@ -5615,13 +5741,13 @@
         <v>6</v>
       </c>
       <c r="C217" s="11" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c r="F217" s="1" t="s">
         <v>49</v>
@@ -5638,10 +5764,10 @@
         <v>220</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E218" s="1" t="s">
-        <v>258</v>
+        <v>11</v>
+      </c>
+      <c r="E218" s="12" t="s">
+        <v>240</v>
       </c>
       <c r="F218" s="1" t="s">
         <v>49</v>
@@ -5658,10 +5784,10 @@
         <v>222</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="F219" s="1" t="s">
         <v>49</v>
@@ -5675,13 +5801,13 @@
         <v>6</v>
       </c>
       <c r="C220" s="11" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>260</v>
+        <v>282</v>
       </c>
       <c r="F220" s="1" t="s">
         <v>49</v>
@@ -5695,15 +5821,815 @@
         <v>6</v>
       </c>
       <c r="C221" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D221" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F221" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B222" s="11">
+        <v>6</v>
+      </c>
+      <c r="C222" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D222" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F222" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B223" s="11">
+        <v>6</v>
+      </c>
+      <c r="C223" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="D221" s="2" t="s">
+      <c r="D223" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B224" s="11">
+        <v>6</v>
+      </c>
+      <c r="C224" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D224" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F224" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B225" s="11">
+        <v>6</v>
+      </c>
+      <c r="C225" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D225" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F225" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B226" s="11">
+        <v>6</v>
+      </c>
+      <c r="C226" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D226" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B227" s="11">
+        <v>6</v>
+      </c>
+      <c r="C227" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D227" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F227" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B228" s="11">
+        <v>6</v>
+      </c>
+      <c r="C228" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D228" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F228" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B229" s="11">
+        <v>6</v>
+      </c>
+      <c r="C229" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D229" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F229" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B230" s="11">
+        <v>6</v>
+      </c>
+      <c r="C230" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D230" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F230" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B231" s="11">
+        <v>6</v>
+      </c>
+      <c r="C231" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D231" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F231" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B232" s="11">
+        <v>6</v>
+      </c>
+      <c r="C232" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D232" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F232" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B233" s="11">
+        <v>6</v>
+      </c>
+      <c r="C233" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D233" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E233" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F233" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B234" s="11">
+        <v>6</v>
+      </c>
+      <c r="C234" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D234" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F234" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A235" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B235" s="11">
+        <v>6</v>
+      </c>
+      <c r="C235" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D235" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B236" s="11">
+        <v>6</v>
+      </c>
+      <c r="C236" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D236" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F236" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A237" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B237" s="11">
+        <v>6</v>
+      </c>
+      <c r="C237" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D237" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F237" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A238" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B238" s="11">
+        <v>6</v>
+      </c>
+      <c r="C238" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D238" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F238" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A239" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B239" s="11">
+        <v>6</v>
+      </c>
+      <c r="C239" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D239" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F239" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A240" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B240" s="11">
+        <v>6</v>
+      </c>
+      <c r="C240" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D240" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E240" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="F240" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B241" s="11">
+        <v>6</v>
+      </c>
+      <c r="C241" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D241" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F241" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B242" s="11">
+        <v>6</v>
+      </c>
+      <c r="C242" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D242" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F242" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A243" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B243" s="11">
+        <v>6</v>
+      </c>
+      <c r="C243" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D243" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F243" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B244" s="11">
+        <v>6</v>
+      </c>
+      <c r="C244" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D244" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F244" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A245" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B245" s="11">
+        <v>6</v>
+      </c>
+      <c r="C245" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D245" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F245" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A246" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B246" s="11">
+        <v>6</v>
+      </c>
+      <c r="C246" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D246" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F246" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A247" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B247" s="11">
+        <v>6</v>
+      </c>
+      <c r="C247" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D247" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F247" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A248" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B248" s="11">
+        <v>6</v>
+      </c>
+      <c r="C248" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D248" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F248" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A249" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B249" s="11">
+        <v>6</v>
+      </c>
+      <c r="C249" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D249" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F249" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A250" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B250" s="11">
+        <v>6</v>
+      </c>
+      <c r="C250" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D250" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F250" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A251" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B251" s="11">
+        <v>6</v>
+      </c>
+      <c r="C251" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D251" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F251" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B252" s="11">
+        <v>6</v>
+      </c>
+      <c r="C252" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D252" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F252" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A253" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B253" s="11">
+        <v>6</v>
+      </c>
+      <c r="C253" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D253" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="F253" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A254" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B254" s="11">
+        <v>6</v>
+      </c>
+      <c r="C254" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D254" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F254" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B255" s="11">
+        <v>6</v>
+      </c>
+      <c r="C255" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D255" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F255" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A256" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B256" s="11">
+        <v>6</v>
+      </c>
+      <c r="C256" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D256" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F256" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A257" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B257" s="11">
+        <v>6</v>
+      </c>
+      <c r="C257" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D257" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F257" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A258" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B258" s="11">
+        <v>6</v>
+      </c>
+      <c r="C258" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D258" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E221" s="1" t="s">
+      <c r="E258" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F258" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A259" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B259" s="11">
+        <v>6</v>
+      </c>
+      <c r="C259" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D259" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E259" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="F221" s="1" t="s">
+      <c r="F259" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B260" s="11">
+        <v>6</v>
+      </c>
+      <c r="C260" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D260" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E260" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F260" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B261" s="11">
+        <v>6</v>
+      </c>
+      <c r="C261" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D261" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F261" s="1" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add US related to "Medicine" and "Nephrology" domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Chain-of-Thought dataset/CoTDataset.xlsx
+++ b/refair-server/datasets/Chain-of-Thought dataset/CoTDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\Chain-of-Thought dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFE0BA4-66D3-405D-B373-6E35A2F9ADDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474458E7-1D78-4EC3-8BF0-F0243EC17D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="346">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -948,6 +948,132 @@
   </si>
   <si>
     <t>As a biomedical researcher, I want to apply word embedding techniques to analyze electronic health records and identify semantic relationships between medical terms (e.g., symptoms, treatments), facilitating more accurate automated diagnosis and treatment recommendation systems.</t>
+  </si>
+  <si>
+    <t>Medicine</t>
+  </si>
+  <si>
+    <t>Nephrology</t>
+  </si>
+  <si>
+    <t>As a medical educator, I want to create a conversational agent using machine learning models to simulate patient interactions for training purposes, allowing medical students to practice clinical decision-making in a controlled environment.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to utilize decision tree algorithms to analyze patient data and identify key risk factors contributing to the development of cardiovascular diseases, to aid in early intervention strategies.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to apply adversarial learning techniques to improve the robustness of MRI image segmentation models, ensuring accurate delineation of tumors and healthy tissues in oncology diagnostics.</t>
+  </si>
+  <si>
+    <t>As a medical technologist, I aim to develop CNN-based algorithms for real-time analysis of electrocardiogram (ECG) signals, assisting clinicians in detecting arrhythmias and other cardiac abnormalities swiftly and accurately.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to develop a document classification model using machine learning to categorize scientific articles into relevant topics such as cardiovascular diseases, oncology, and neurology, facilitating easier literature review and research synthesis.</t>
+  </si>
+  <si>
+    <t>As a clinical researcher, I want to utilize entity extraction models in natural language processing to identify and extract key clinical parameters such as symptoms, treatment outcomes, and patient demographics from unstructured clinical notes, enabling comprehensive data analysis and clinical decision support.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to employ feature selection techniques in machine learning to identify the most relevant biomarkers from genetic data, aiding in the early detection of hereditary diseases and informing personalized treatment strategies.</t>
+  </si>
+  <si>
+    <t>As a clinical researcher, I aim to address class imbalance in medical diagnostic datasets by applying sampling techniques such as SMOTE (Synthetic Minority Over-sampling Technique) to improve the sensitivity and specificity of diagnostic models for detecting rare conditions with limited data availability.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to develop a keyword extraction model using natural language processing (NLP) techniques to automatically identify key medical terminologies from patient discharge summaries, facilitating quicker information retrieval and medical record abstraction.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I want to implement a KNN algorithm to predict patient readmission risks based on demographic data, medical history, and recent hospitalization records, enabling proactive patient management and resource allocation.</t>
+  </si>
+  <si>
+    <t>As a nephrology clinician, I seek to utilize k-NN algorithms to identify suitable kidney donor matches based on compatibility metrics derived from donor and recipient profiles, optimizing transplant outcomes.</t>
+  </si>
+  <si>
+    <t>As a clinical researcher, I want to develop a multi-label classification model using machine learning to predict the presence of multiple comorbidities in diabetic patients based on their medical history and diagnostic test results, enabling personalized treatment plans and risk management strategies.</t>
+  </si>
+  <si>
+    <t>As a healthcare informatician, I want to implement a neural network-based natural language processing (NLP) model to extract clinical insights and predict patient outcomes from unstructured clinical notes and EHRs, supporting clinical decision-making and care coordination across healthcare settings.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to build a random forest model to predict patient outcomes after cardiac surgery by analyzing a combination of clinical variables such as age, comorbidities, and surgical complications, aiding in post-operative care planning and patient management.</t>
+  </si>
+  <si>
+    <t>As a clinical researcher, I want to use semantic similarity measures to compare and cluster electronic health records (EHRs) based on patient histories and medical conditions, identifying cohorts for clinical trials and retrospective studies efficiently.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to apply sentiment analysis techniques to analyze sentiment trends in medical literature and academic publications related to specific treatments or therapies, to understand the overall reception and impact of new medical advancements within the scientific community.</t>
+  </si>
+  <si>
+    <t>As a clinical researcher, I want to use speech-to-text technology to transcribe and analyze audio recordings of patient interviews and focus group discussions, enabling qualitative data analysis and deeper insights into patient experiences and perspectives on healthcare interventions.</t>
+  </si>
+  <si>
+    <t>As a medical librarian, I want to develop a text categorization system using natural language processing (NLP) to classify research articles and clinical studies into relevant medical specialties such as cardiology, oncology, and neurology, facilitating efficient literature review and knowledge discovery for healthcare professionals.</t>
+  </si>
+  <si>
+    <t>As a clinical researcher, I want to apply unsupervised clustering algorithms to analyze patient electronic health records (EHRs) and identify distinct patient phenotypes or disease subtypes based on clinical characteristics and treatment responses, facilitating personalized medicine approaches and targeted interventions.</t>
+  </si>
+  <si>
+    <t>As a nephrology researcher, I aim to apply unsupervised clustering algorithms to patient electronic health records to identify distinct phenotypic clusters of chronic kidney disease progression, uncovering novel disease subtypes and their clinical implications.</t>
+  </si>
+  <si>
+    <t>As a medical educator, I intend to implement voice recognition tools in virtual simulation environments for medical training, allowing students to practice patient interactions and clinical decision-making skills in realistic scenarios with automated feedback.</t>
+  </si>
+  <si>
+    <t>As a nephrology researcher, I aim to use adversarial learning techniques to enhance the robustness of kidney disease classification models against adversarial attacks, ensuring reliable predictions even in the presence of maliciously crafted input data.</t>
+  </si>
+  <si>
+    <t>As a nephrology informatics specialist, I want to apply CNN models to analyze renal ultrasound images and detect early signs of kidney abnormalities such as cysts or tumors, enabling timely intervention and treatment planning.</t>
+  </si>
+  <si>
+    <t>As a nephrology clinician, I want to develop a conversational agent that can engage with patients to gather dietary habits and fluid intake data, utilizing machine learning to personalize dietary recommendations for kidney health.</t>
+  </si>
+  <si>
+    <t>As a nephrology clinician, I want to utilize decision tree models to predict the risk of kidney transplant rejection based on patient demographics, medical history, and immunosuppressant drug dosages, facilitating proactive adjustments in treatment plans.</t>
+  </si>
+  <si>
+    <t>As a nephrology researcher, I aim to develop a document classification system that categorizes research papers into topics such as glomerular diseases, renal transplantation, and chronic kidney disease stages, facilitating targeted literature reviews and research synthesis.</t>
+  </si>
+  <si>
+    <t>As a nephrology clinician, I seek to implement an entity extraction model that identifies dietary habits and fluid intake patterns from patient records, aiding in the assessment of dietary influences on kidney health and the customization of nutritional counseling.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider specializing in nephrology, I propose using feature selection methods to streamline the analysis of patient electronic health records, identifying key risk factors for acute kidney injury to guide preventive interventions.</t>
+  </si>
+  <si>
+    <t>As a nephrology researcher, I aim to address class imbalance in patient datasets related to rare kidney diseases using oversampling techniques, ensuring that machine learning models are trained effectively to recognize and diagnose these conditions early.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider specializing in nephrology, I want to implement a keyword extraction system that automatically identifies key symptoms and diagnostic criteria from patient clinical notes, aiding in accurate and timely diagnosis of kidney diseases.</t>
+  </si>
+  <si>
+    <t>As a nephrology researcher, I aim to develop a multi-label classification model that predicts the presence of multiple co-occurring kidney diseases (e.g., diabetic nephropathy, glomerulonephritis) based on patient clinical profiles and genetic markers, supporting personalized treatment plans.</t>
+  </si>
+  <si>
+    <t>As a nephrology researcher, I aim to develop a neural network architecture that analyzes histopathological images of kidney biopsies to classify different types of renal diseases (e.g., nephrotic syndrome, tubulointerstitial nephritis) with high accuracy, aiding pathologists in diagnosis.</t>
+  </si>
+  <si>
+    <t>As a nephrology researcher, I aim to develop a random forest model that predicts the progression of chronic kidney disease stages based on patient demographics, laboratory results, and treatment histories, facilitating personalized patient management plans.</t>
+  </si>
+  <si>
+    <t>As a nephrology researcher, I aim to develop a semantic similarity algorithm to compare clinical trial protocols related to kidney disease treatments, facilitating the identification of similar study designs and enhancing research collaboration.</t>
+  </si>
+  <si>
+    <t>As a nephrology researcher, I aim to develop a sentiment analysis tool to analyze patient feedback from renal care satisfaction surveys, identifying positive and negative sentiments towards healthcare services to improve patient experience.</t>
+  </si>
+  <si>
+    <t>As a nephrology clinician, I seek to utilize speech-to-text technology to document real-time observations and treatment plans during rounds and patient visits, enhancing communication among healthcare teams and ensuring timely patient care updates.</t>
+  </si>
+  <si>
+    <t>As a nephrology researcher, I aim to develop a text categorization model that classifies research articles and clinical guidelines into relevant nephrology subfields (e.g., glomerular diseases, dialysis modalities), facilitating efficient literature review and knowledge synthesis.</t>
+  </si>
+  <si>
+    <t>As a nephrology researcher, I aim to develop a voice recognition system that transcribes nephrology lectures and conferences into text, facilitating efficient knowledge dissemination and accessibility for healthcare professionals and researchers.</t>
+  </si>
+  <si>
+    <t>As a nephrology clinician, I seek to utilize word embedding techniques to cluster patient electronic health records based on similar clinical features and treatment responses, enabling personalized treatment planning and predictive analytics for chronic kidney disease management.</t>
+  </si>
+  <si>
+    <t>As a clinical data scientist, I aim to use word embedding models to analyze patient notes and medical records to identify patterns in disease progression and treatment outcomes, enabling personalized medicine approaches and predictive analytics in healthcare settings.</t>
   </si>
 </sst>
 </file>
@@ -1044,7 +1170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1062,7 +1188,13 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1398,10 +1530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F261"/>
+  <dimension ref="A1:F301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E236" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F221" sqref="F221:F261"/>
+    <sheetView tabSelected="1" topLeftCell="A277" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E300" sqref="E300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5046,7 +5178,7 @@
       <c r="D182" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E182" s="1" t="s">
+      <c r="E182" s="12" t="s">
         <v>221</v>
       </c>
       <c r="F182" s="1" t="s">
@@ -5066,7 +5198,7 @@
       <c r="D183" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E183" s="1" t="s">
+      <c r="E183" s="12" t="s">
         <v>223</v>
       </c>
       <c r="F183" s="1" t="s">
@@ -5086,7 +5218,7 @@
       <c r="D184" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E184" s="1" t="s">
+      <c r="E184" s="12" t="s">
         <v>263</v>
       </c>
       <c r="F184" s="1" t="s">
@@ -5106,7 +5238,7 @@
       <c r="D185" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E185" s="1" t="s">
+      <c r="E185" s="12" t="s">
         <v>265</v>
       </c>
       <c r="F185" s="1" t="s">
@@ -5121,13 +5253,13 @@
         <v>6</v>
       </c>
       <c r="C186" s="11" t="s">
-        <v>220</v>
+        <v>304</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>224</v>
+        <v>17</v>
+      </c>
+      <c r="E186" s="12" t="s">
+        <v>308</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>49</v>
@@ -5141,13 +5273,13 @@
         <v>6</v>
       </c>
       <c r="C187" s="11" t="s">
-        <v>222</v>
+        <v>305</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E187" s="1" t="s">
-        <v>225</v>
+        <v>17</v>
+      </c>
+      <c r="E187" s="12" t="s">
+        <v>327</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>49</v>
@@ -5161,13 +5293,13 @@
         <v>6</v>
       </c>
       <c r="C188" s="11" t="s">
-        <v>262</v>
+        <v>220</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E188" s="1" t="s">
-        <v>266</v>
+      <c r="E188" s="12" t="s">
+        <v>224</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>49</v>
@@ -5181,13 +5313,13 @@
         <v>6</v>
       </c>
       <c r="C189" s="11" t="s">
-        <v>264</v>
+        <v>222</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E189" s="1" t="s">
-        <v>267</v>
+      <c r="E189" s="12" t="s">
+        <v>225</v>
       </c>
       <c r="F189" s="1" t="s">
         <v>49</v>
@@ -5201,13 +5333,13 @@
         <v>6</v>
       </c>
       <c r="C190" s="11" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E190" s="1" t="s">
-        <v>226</v>
+        <v>25</v>
+      </c>
+      <c r="E190" s="12" t="s">
+        <v>266</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>49</v>
@@ -5221,13 +5353,13 @@
         <v>6</v>
       </c>
       <c r="C191" s="11" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E191" s="1" t="s">
-        <v>227</v>
+        <v>25</v>
+      </c>
+      <c r="E191" s="12" t="s">
+        <v>267</v>
       </c>
       <c r="F191" s="1" t="s">
         <v>49</v>
@@ -5241,13 +5373,13 @@
         <v>6</v>
       </c>
       <c r="C192" s="11" t="s">
-        <v>262</v>
+        <v>304</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E192" s="1" t="s">
-        <v>268</v>
+        <v>25</v>
+      </c>
+      <c r="E192" s="12" t="s">
+        <v>309</v>
       </c>
       <c r="F192" s="1" t="s">
         <v>49</v>
@@ -5261,13 +5393,13 @@
         <v>6</v>
       </c>
       <c r="C193" s="11" t="s">
-        <v>264</v>
+        <v>305</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E193" s="1" t="s">
-        <v>269</v>
+        <v>25</v>
+      </c>
+      <c r="E193" s="12" t="s">
+        <v>328</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>49</v>
@@ -5284,10 +5416,10 @@
         <v>220</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E194" s="1" t="s">
-        <v>228</v>
+        <v>18</v>
+      </c>
+      <c r="E194" s="12" t="s">
+        <v>226</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>49</v>
@@ -5304,10 +5436,10 @@
         <v>222</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E195" s="1" t="s">
-        <v>229</v>
+        <v>18</v>
+      </c>
+      <c r="E195" s="12" t="s">
+        <v>227</v>
       </c>
       <c r="F195" s="1" t="s">
         <v>49</v>
@@ -5324,10 +5456,10 @@
         <v>262</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E196" s="1" t="s">
-        <v>270</v>
+        <v>18</v>
+      </c>
+      <c r="E196" s="12" t="s">
+        <v>268</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>49</v>
@@ -5344,10 +5476,10 @@
         <v>264</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E197" s="1" t="s">
-        <v>271</v>
+        <v>18</v>
+      </c>
+      <c r="E197" s="12" t="s">
+        <v>269</v>
       </c>
       <c r="F197" s="1" t="s">
         <v>49</v>
@@ -5361,13 +5493,13 @@
         <v>6</v>
       </c>
       <c r="C198" s="11" t="s">
-        <v>220</v>
+        <v>304</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E198" s="1" t="s">
-        <v>230</v>
+        <v>18</v>
+      </c>
+      <c r="E198" s="12" t="s">
+        <v>306</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>49</v>
@@ -5381,13 +5513,13 @@
         <v>6</v>
       </c>
       <c r="C199" s="11" t="s">
-        <v>222</v>
+        <v>305</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E199" s="1" t="s">
-        <v>231</v>
+        <v>18</v>
+      </c>
+      <c r="E199" s="13" t="s">
+        <v>329</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>49</v>
@@ -5401,13 +5533,13 @@
         <v>6</v>
       </c>
       <c r="C200" s="11" t="s">
-        <v>262</v>
+        <v>220</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E200" s="1" t="s">
-        <v>272</v>
+        <v>9</v>
+      </c>
+      <c r="E200" s="12" t="s">
+        <v>228</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>49</v>
@@ -5421,13 +5553,13 @@
         <v>6</v>
       </c>
       <c r="C201" s="11" t="s">
-        <v>264</v>
+        <v>222</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E201" s="1" t="s">
-        <v>273</v>
+        <v>9</v>
+      </c>
+      <c r="E201" s="12" t="s">
+        <v>229</v>
       </c>
       <c r="F201" s="1" t="s">
         <v>49</v>
@@ -5441,13 +5573,13 @@
         <v>6</v>
       </c>
       <c r="C202" s="11" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E202" s="1" t="s">
-        <v>232</v>
+        <v>9</v>
+      </c>
+      <c r="E202" s="12" t="s">
+        <v>270</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>49</v>
@@ -5461,13 +5593,13 @@
         <v>6</v>
       </c>
       <c r="C203" s="11" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E203" s="1" t="s">
-        <v>233</v>
+        <v>9</v>
+      </c>
+      <c r="E203" s="12" t="s">
+        <v>271</v>
       </c>
       <c r="F203" s="1" t="s">
         <v>49</v>
@@ -5481,13 +5613,13 @@
         <v>6</v>
       </c>
       <c r="C204" s="11" t="s">
-        <v>262</v>
+        <v>304</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E204" s="1" t="s">
-        <v>274</v>
+        <v>9</v>
+      </c>
+      <c r="E204" s="12" t="s">
+        <v>307</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>49</v>
@@ -5501,13 +5633,13 @@
         <v>6</v>
       </c>
       <c r="C205" s="11" t="s">
-        <v>264</v>
+        <v>305</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E205" s="1" t="s">
-        <v>275</v>
+        <v>9</v>
+      </c>
+      <c r="E205" s="12" t="s">
+        <v>330</v>
       </c>
       <c r="F205" s="1" t="s">
         <v>49</v>
@@ -5524,10 +5656,10 @@
         <v>220</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E206" s="1" t="s">
-        <v>234</v>
+        <v>26</v>
+      </c>
+      <c r="E206" s="12" t="s">
+        <v>230</v>
       </c>
       <c r="F206" s="1" t="s">
         <v>49</v>
@@ -5544,10 +5676,10 @@
         <v>222</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E207" s="1" t="s">
-        <v>235</v>
+        <v>26</v>
+      </c>
+      <c r="E207" s="12" t="s">
+        <v>231</v>
       </c>
       <c r="F207" s="1" t="s">
         <v>49</v>
@@ -5564,10 +5696,10 @@
         <v>262</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E208" s="1" t="s">
-        <v>276</v>
+        <v>26</v>
+      </c>
+      <c r="E208" s="12" t="s">
+        <v>272</v>
       </c>
       <c r="F208" s="1" t="s">
         <v>49</v>
@@ -5584,10 +5716,10 @@
         <v>264</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E209" s="1" t="s">
-        <v>277</v>
+        <v>26</v>
+      </c>
+      <c r="E209" s="12" t="s">
+        <v>273</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>49</v>
@@ -5601,13 +5733,13 @@
         <v>6</v>
       </c>
       <c r="C210" s="11" t="s">
-        <v>220</v>
+        <v>304</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E210" s="1" t="s">
-        <v>236</v>
+        <v>26</v>
+      </c>
+      <c r="E210" s="12" t="s">
+        <v>310</v>
       </c>
       <c r="F210" s="1" t="s">
         <v>49</v>
@@ -5621,13 +5753,13 @@
         <v>6</v>
       </c>
       <c r="C211" s="11" t="s">
-        <v>222</v>
+        <v>305</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E211" s="1" t="s">
-        <v>237</v>
+        <v>26</v>
+      </c>
+      <c r="E211" s="13" t="s">
+        <v>331</v>
       </c>
       <c r="F211" s="1" t="s">
         <v>49</v>
@@ -5641,13 +5773,13 @@
         <v>6</v>
       </c>
       <c r="C212" s="11" t="s">
-        <v>262</v>
+        <v>220</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>278</v>
+        <v>20</v>
+      </c>
+      <c r="E212" s="12" t="s">
+        <v>232</v>
       </c>
       <c r="F212" s="1" t="s">
         <v>49</v>
@@ -5661,13 +5793,13 @@
         <v>6</v>
       </c>
       <c r="C213" s="11" t="s">
-        <v>264</v>
+        <v>222</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E213" s="1" t="s">
-        <v>279</v>
+        <v>20</v>
+      </c>
+      <c r="E213" s="12" t="s">
+        <v>233</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>49</v>
@@ -5681,13 +5813,13 @@
         <v>6</v>
       </c>
       <c r="C214" s="11" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E214" s="1" t="s">
-        <v>238</v>
+        <v>20</v>
+      </c>
+      <c r="E214" s="12" t="s">
+        <v>274</v>
       </c>
       <c r="F214" s="1" t="s">
         <v>49</v>
@@ -5701,13 +5833,13 @@
         <v>6</v>
       </c>
       <c r="C215" s="11" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E215" s="1" t="s">
-        <v>239</v>
+        <v>20</v>
+      </c>
+      <c r="E215" s="12" t="s">
+        <v>275</v>
       </c>
       <c r="F215" s="1" t="s">
         <v>49</v>
@@ -5721,13 +5853,13 @@
         <v>6</v>
       </c>
       <c r="C216" s="11" t="s">
-        <v>262</v>
+        <v>304</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E216" s="1" t="s">
-        <v>280</v>
+        <v>20</v>
+      </c>
+      <c r="E216" s="12" t="s">
+        <v>311</v>
       </c>
       <c r="F216" s="1" t="s">
         <v>49</v>
@@ -5741,13 +5873,13 @@
         <v>6</v>
       </c>
       <c r="C217" s="11" t="s">
-        <v>264</v>
+        <v>305</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E217" s="1" t="s">
-        <v>281</v>
+        <v>20</v>
+      </c>
+      <c r="E217" s="13" t="s">
+        <v>332</v>
       </c>
       <c r="F217" s="1" t="s">
         <v>49</v>
@@ -5764,10 +5896,10 @@
         <v>220</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E218" s="12" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F218" s="1" t="s">
         <v>49</v>
@@ -5784,10 +5916,10 @@
         <v>222</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E219" s="1" t="s">
-        <v>241</v>
+        <v>22</v>
+      </c>
+      <c r="E219" s="12" t="s">
+        <v>235</v>
       </c>
       <c r="F219" s="1" t="s">
         <v>49</v>
@@ -5804,10 +5936,10 @@
         <v>262</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E220" s="1" t="s">
-        <v>282</v>
+        <v>22</v>
+      </c>
+      <c r="E220" s="12" t="s">
+        <v>276</v>
       </c>
       <c r="F220" s="1" t="s">
         <v>49</v>
@@ -5824,10 +5956,10 @@
         <v>264</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>283</v>
+        <v>22</v>
+      </c>
+      <c r="E221" s="12" t="s">
+        <v>277</v>
       </c>
       <c r="F221" s="1" t="s">
         <v>49</v>
@@ -5841,13 +5973,13 @@
         <v>6</v>
       </c>
       <c r="C222" s="11" t="s">
-        <v>220</v>
+        <v>304</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E222" s="1" t="s">
-        <v>242</v>
+        <v>22</v>
+      </c>
+      <c r="E222" s="12" t="s">
+        <v>312</v>
       </c>
       <c r="F222" s="1" t="s">
         <v>49</v>
@@ -5861,13 +5993,13 @@
         <v>6</v>
       </c>
       <c r="C223" s="11" t="s">
-        <v>222</v>
+        <v>305</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E223" s="1" t="s">
-        <v>243</v>
+        <v>22</v>
+      </c>
+      <c r="E223" s="12" t="s">
+        <v>333</v>
       </c>
       <c r="F223" s="1" t="s">
         <v>49</v>
@@ -5881,13 +6013,13 @@
         <v>6</v>
       </c>
       <c r="C224" s="11" t="s">
-        <v>262</v>
+        <v>220</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E224" s="1" t="s">
-        <v>284</v>
+        <v>10</v>
+      </c>
+      <c r="E224" s="12" t="s">
+        <v>236</v>
       </c>
       <c r="F224" s="1" t="s">
         <v>49</v>
@@ -5901,13 +6033,13 @@
         <v>6</v>
       </c>
       <c r="C225" s="11" t="s">
-        <v>264</v>
+        <v>222</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E225" s="1" t="s">
-        <v>285</v>
+        <v>10</v>
+      </c>
+      <c r="E225" s="12" t="s">
+        <v>237</v>
       </c>
       <c r="F225" s="1" t="s">
         <v>49</v>
@@ -5921,13 +6053,13 @@
         <v>6</v>
       </c>
       <c r="C226" s="11" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E226" s="1" t="s">
-        <v>244</v>
+        <v>10</v>
+      </c>
+      <c r="E226" s="12" t="s">
+        <v>278</v>
       </c>
       <c r="F226" s="1" t="s">
         <v>49</v>
@@ -5941,13 +6073,13 @@
         <v>6</v>
       </c>
       <c r="C227" s="11" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E227" s="1" t="s">
-        <v>245</v>
+        <v>10</v>
+      </c>
+      <c r="E227" s="12" t="s">
+        <v>279</v>
       </c>
       <c r="F227" s="1" t="s">
         <v>49</v>
@@ -5961,13 +6093,13 @@
         <v>6</v>
       </c>
       <c r="C228" s="11" t="s">
-        <v>262</v>
+        <v>304</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E228" s="1" t="s">
-        <v>286</v>
+        <v>10</v>
+      </c>
+      <c r="E228" s="12" t="s">
+        <v>313</v>
       </c>
       <c r="F228" s="1" t="s">
         <v>49</v>
@@ -5981,13 +6113,13 @@
         <v>6</v>
       </c>
       <c r="C229" s="11" t="s">
-        <v>264</v>
+        <v>305</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E229" s="1" t="s">
-        <v>287</v>
+        <v>10</v>
+      </c>
+      <c r="E229" s="12" t="s">
+        <v>334</v>
       </c>
       <c r="F229" s="1" t="s">
         <v>49</v>
@@ -6004,10 +6136,10 @@
         <v>220</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E230" s="1" t="s">
-        <v>246</v>
+        <v>21</v>
+      </c>
+      <c r="E230" s="12" t="s">
+        <v>238</v>
       </c>
       <c r="F230" s="1" t="s">
         <v>49</v>
@@ -6024,10 +6156,10 @@
         <v>222</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E231" s="1" t="s">
-        <v>247</v>
+        <v>21</v>
+      </c>
+      <c r="E231" s="12" t="s">
+        <v>239</v>
       </c>
       <c r="F231" s="1" t="s">
         <v>49</v>
@@ -6044,10 +6176,10 @@
         <v>262</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E232" s="1" t="s">
-        <v>288</v>
+        <v>21</v>
+      </c>
+      <c r="E232" s="12" t="s">
+        <v>280</v>
       </c>
       <c r="F232" s="1" t="s">
         <v>49</v>
@@ -6064,10 +6196,10 @@
         <v>264</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E233" s="1" t="s">
-        <v>289</v>
+        <v>21</v>
+      </c>
+      <c r="E233" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="F233" s="1" t="s">
         <v>49</v>
@@ -6081,13 +6213,13 @@
         <v>6</v>
       </c>
       <c r="C234" s="11" t="s">
-        <v>220</v>
+        <v>304</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E234" s="1" t="s">
-        <v>248</v>
+        <v>21</v>
+      </c>
+      <c r="E234" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="F234" s="1" t="s">
         <v>49</v>
@@ -6101,13 +6233,13 @@
         <v>6</v>
       </c>
       <c r="C235" s="11" t="s">
-        <v>222</v>
+        <v>305</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E235" s="1" t="s">
-        <v>249</v>
+        <v>21</v>
+      </c>
+      <c r="E235" s="12" t="s">
+        <v>335</v>
       </c>
       <c r="F235" s="1" t="s">
         <v>49</v>
@@ -6121,13 +6253,13 @@
         <v>6</v>
       </c>
       <c r="C236" s="11" t="s">
-        <v>262</v>
+        <v>220</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>290</v>
+        <v>11</v>
+      </c>
+      <c r="E236" s="14" t="s">
+        <v>240</v>
       </c>
       <c r="F236" s="1" t="s">
         <v>49</v>
@@ -6141,13 +6273,13 @@
         <v>6</v>
       </c>
       <c r="C237" s="11" t="s">
-        <v>264</v>
+        <v>222</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E237" s="1" t="s">
-        <v>291</v>
+        <v>11</v>
+      </c>
+      <c r="E237" s="12" t="s">
+        <v>241</v>
       </c>
       <c r="F237" s="1" t="s">
         <v>49</v>
@@ -6161,13 +6293,13 @@
         <v>6</v>
       </c>
       <c r="C238" s="11" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E238" s="1" t="s">
-        <v>250</v>
+        <v>11</v>
+      </c>
+      <c r="E238" s="12" t="s">
+        <v>282</v>
       </c>
       <c r="F238" s="1" t="s">
         <v>49</v>
@@ -6181,13 +6313,13 @@
         <v>6</v>
       </c>
       <c r="C239" s="11" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E239" s="1" t="s">
-        <v>251</v>
+        <v>11</v>
+      </c>
+      <c r="E239" s="12" t="s">
+        <v>283</v>
       </c>
       <c r="F239" s="1" t="s">
         <v>49</v>
@@ -6201,13 +6333,13 @@
         <v>6</v>
       </c>
       <c r="C240" s="11" t="s">
-        <v>262</v>
+        <v>304</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E240" s="1" t="s">
-        <v>292</v>
+        <v>11</v>
+      </c>
+      <c r="E240" s="12" t="s">
+        <v>315</v>
       </c>
       <c r="F240" s="1" t="s">
         <v>49</v>
@@ -6221,13 +6353,13 @@
         <v>6</v>
       </c>
       <c r="C241" s="11" t="s">
-        <v>264</v>
+        <v>305</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E241" s="1" t="s">
-        <v>293</v>
+        <v>11</v>
+      </c>
+      <c r="E241" s="12" t="s">
+        <v>316</v>
       </c>
       <c r="F241" s="1" t="s">
         <v>49</v>
@@ -6244,10 +6376,10 @@
         <v>220</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E242" s="1" t="s">
-        <v>252</v>
+        <v>24</v>
+      </c>
+      <c r="E242" s="12" t="s">
+        <v>242</v>
       </c>
       <c r="F242" s="1" t="s">
         <v>49</v>
@@ -6264,10 +6396,10 @@
         <v>222</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E243" s="1" t="s">
-        <v>253</v>
+        <v>24</v>
+      </c>
+      <c r="E243" s="12" t="s">
+        <v>243</v>
       </c>
       <c r="F243" s="1" t="s">
         <v>49</v>
@@ -6284,10 +6416,10 @@
         <v>262</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E244" s="1" t="s">
-        <v>294</v>
+        <v>24</v>
+      </c>
+      <c r="E244" s="12" t="s">
+        <v>284</v>
       </c>
       <c r="F244" s="1" t="s">
         <v>49</v>
@@ -6304,10 +6436,10 @@
         <v>264</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E245" s="1" t="s">
-        <v>295</v>
+        <v>24</v>
+      </c>
+      <c r="E245" s="12" t="s">
+        <v>285</v>
       </c>
       <c r="F245" s="1" t="s">
         <v>49</v>
@@ -6321,13 +6453,13 @@
         <v>6</v>
       </c>
       <c r="C246" s="11" t="s">
-        <v>220</v>
+        <v>304</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>254</v>
+        <v>24</v>
+      </c>
+      <c r="E246" s="12" t="s">
+        <v>317</v>
       </c>
       <c r="F246" s="1" t="s">
         <v>49</v>
@@ -6341,13 +6473,13 @@
         <v>6</v>
       </c>
       <c r="C247" s="11" t="s">
-        <v>222</v>
+        <v>305</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E247" s="1" t="s">
-        <v>255</v>
+        <v>24</v>
+      </c>
+      <c r="E247" s="12" t="s">
+        <v>336</v>
       </c>
       <c r="F247" s="1" t="s">
         <v>49</v>
@@ -6361,13 +6493,13 @@
         <v>6</v>
       </c>
       <c r="C248" s="11" t="s">
-        <v>262</v>
+        <v>220</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E248" s="1" t="s">
-        <v>296</v>
+        <v>12</v>
+      </c>
+      <c r="E248" s="12" t="s">
+        <v>244</v>
       </c>
       <c r="F248" s="1" t="s">
         <v>49</v>
@@ -6381,13 +6513,13 @@
         <v>6</v>
       </c>
       <c r="C249" s="11" t="s">
-        <v>264</v>
+        <v>222</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E249" s="1" t="s">
-        <v>297</v>
+        <v>12</v>
+      </c>
+      <c r="E249" s="12" t="s">
+        <v>245</v>
       </c>
       <c r="F249" s="1" t="s">
         <v>49</v>
@@ -6401,13 +6533,13 @@
         <v>6</v>
       </c>
       <c r="C250" s="11" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>256</v>
+        <v>12</v>
+      </c>
+      <c r="E250" s="12" t="s">
+        <v>286</v>
       </c>
       <c r="F250" s="1" t="s">
         <v>49</v>
@@ -6421,13 +6553,13 @@
         <v>6</v>
       </c>
       <c r="C251" s="11" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E251" s="1" t="s">
-        <v>257</v>
+        <v>12</v>
+      </c>
+      <c r="E251" s="12" t="s">
+        <v>287</v>
       </c>
       <c r="F251" s="1" t="s">
         <v>49</v>
@@ -6441,13 +6573,13 @@
         <v>6</v>
       </c>
       <c r="C252" s="11" t="s">
-        <v>262</v>
+        <v>304</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E252" s="1" t="s">
-        <v>298</v>
+        <v>12</v>
+      </c>
+      <c r="E252" s="12" t="s">
+        <v>318</v>
       </c>
       <c r="F252" s="1" t="s">
         <v>49</v>
@@ -6461,13 +6593,13 @@
         <v>6</v>
       </c>
       <c r="C253" s="11" t="s">
-        <v>264</v>
+        <v>305</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E253" s="1" t="s">
-        <v>299</v>
+        <v>12</v>
+      </c>
+      <c r="E253" s="12" t="s">
+        <v>337</v>
       </c>
       <c r="F253" s="1" t="s">
         <v>49</v>
@@ -6484,10 +6616,10 @@
         <v>220</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E254" s="1" t="s">
-        <v>258</v>
+        <v>13</v>
+      </c>
+      <c r="E254" s="12" t="s">
+        <v>246</v>
       </c>
       <c r="F254" s="1" t="s">
         <v>49</v>
@@ -6504,10 +6636,10 @@
         <v>222</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E255" s="1" t="s">
-        <v>259</v>
+        <v>13</v>
+      </c>
+      <c r="E255" s="12" t="s">
+        <v>247</v>
       </c>
       <c r="F255" s="1" t="s">
         <v>49</v>
@@ -6524,10 +6656,10 @@
         <v>262</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E256" s="1" t="s">
-        <v>300</v>
+        <v>13</v>
+      </c>
+      <c r="E256" s="12" t="s">
+        <v>288</v>
       </c>
       <c r="F256" s="1" t="s">
         <v>49</v>
@@ -6544,10 +6676,10 @@
         <v>264</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E257" s="1" t="s">
-        <v>301</v>
+        <v>13</v>
+      </c>
+      <c r="E257" s="12" t="s">
+        <v>289</v>
       </c>
       <c r="F257" s="1" t="s">
         <v>49</v>
@@ -6561,13 +6693,13 @@
         <v>6</v>
       </c>
       <c r="C258" s="11" t="s">
-        <v>220</v>
+        <v>304</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E258" s="1" t="s">
-        <v>260</v>
+        <v>13</v>
+      </c>
+      <c r="E258" s="12" t="s">
+        <v>319</v>
       </c>
       <c r="F258" s="1" t="s">
         <v>49</v>
@@ -6581,13 +6713,13 @@
         <v>6</v>
       </c>
       <c r="C259" s="11" t="s">
-        <v>222</v>
+        <v>305</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E259" s="1" t="s">
-        <v>261</v>
+        <v>13</v>
+      </c>
+      <c r="E259" s="12" t="s">
+        <v>338</v>
       </c>
       <c r="F259" s="1" t="s">
         <v>49</v>
@@ -6601,13 +6733,13 @@
         <v>6</v>
       </c>
       <c r="C260" s="11" t="s">
-        <v>262</v>
+        <v>220</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E260" s="1" t="s">
-        <v>302</v>
+        <v>14</v>
+      </c>
+      <c r="E260" s="12" t="s">
+        <v>248</v>
       </c>
       <c r="F260" s="1" t="s">
         <v>49</v>
@@ -6621,15 +6753,815 @@
         <v>6</v>
       </c>
       <c r="C261" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D261" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E261" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="F261" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B262" s="11">
+        <v>6</v>
+      </c>
+      <c r="C262" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D262" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E262" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="F262" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A263" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B263" s="11">
+        <v>6</v>
+      </c>
+      <c r="C263" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="D261" s="2" t="s">
+      <c r="D263" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E263" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="F263" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A264" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B264" s="11">
+        <v>6</v>
+      </c>
+      <c r="C264" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="D264" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E264" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="F264" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B265" s="11">
+        <v>6</v>
+      </c>
+      <c r="C265" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="D265" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E265" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="F265" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B266" s="11">
+        <v>6</v>
+      </c>
+      <c r="C266" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D266" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E266" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="F266" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B267" s="11">
+        <v>6</v>
+      </c>
+      <c r="C267" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D267" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E267" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="F267" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B268" s="11">
+        <v>6</v>
+      </c>
+      <c r="C268" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D268" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E268" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="F268" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B269" s="11">
+        <v>6</v>
+      </c>
+      <c r="C269" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D269" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E269" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="F269" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B270" s="11">
+        <v>6</v>
+      </c>
+      <c r="C270" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="D270" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E270" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="F270" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B271" s="11">
+        <v>6</v>
+      </c>
+      <c r="C271" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="D271" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E271" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="F271" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A272" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B272" s="11">
+        <v>6</v>
+      </c>
+      <c r="C272" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D272" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E272" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="F272" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A273" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B273" s="11">
+        <v>6</v>
+      </c>
+      <c r="C273" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D273" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E273" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="F273" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A274" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B274" s="11">
+        <v>6</v>
+      </c>
+      <c r="C274" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D274" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E274" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="F274" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A275" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B275" s="11">
+        <v>6</v>
+      </c>
+      <c r="C275" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D275" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E275" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="F275" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A276" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B276" s="11">
+        <v>6</v>
+      </c>
+      <c r="C276" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="D276" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E276" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="F276" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A277" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B277" s="11">
+        <v>6</v>
+      </c>
+      <c r="C277" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="D277" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E277" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="F277" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A278" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B278" s="11">
+        <v>6</v>
+      </c>
+      <c r="C278" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D278" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E278" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="F278" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B279" s="11">
+        <v>6</v>
+      </c>
+      <c r="C279" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D279" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E279" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="F279" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A280" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B280" s="11">
+        <v>6</v>
+      </c>
+      <c r="C280" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D280" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E280" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="F280" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A281" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B281" s="11">
+        <v>6</v>
+      </c>
+      <c r="C281" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D281" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E281" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="F281" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A282" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B282" s="11">
+        <v>6</v>
+      </c>
+      <c r="C282" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="D282" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E282" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="F282" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A283" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B283" s="11">
+        <v>6</v>
+      </c>
+      <c r="C283" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="D283" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E283" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="F283" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A284" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B284" s="11">
+        <v>6</v>
+      </c>
+      <c r="C284" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D284" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E284" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="F284" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A285" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B285" s="11">
+        <v>6</v>
+      </c>
+      <c r="C285" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D285" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E285" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="F285" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A286" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B286" s="11">
+        <v>6</v>
+      </c>
+      <c r="C286" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D286" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E286" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="F286" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A287" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B287" s="11">
+        <v>6</v>
+      </c>
+      <c r="C287" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D287" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E287" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="F287" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A288" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B288" s="11">
+        <v>6</v>
+      </c>
+      <c r="C288" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="D288" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E288" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="F288" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A289" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B289" s="11">
+        <v>6</v>
+      </c>
+      <c r="C289" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="D289" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E289" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="F289" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A290" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B290" s="11">
+        <v>6</v>
+      </c>
+      <c r="C290" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D290" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E290" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="F290" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A291" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B291" s="11">
+        <v>6</v>
+      </c>
+      <c r="C291" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D291" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E291" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="F291" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A292" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B292" s="11">
+        <v>6</v>
+      </c>
+      <c r="C292" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D292" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E292" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="F292" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A293" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B293" s="11">
+        <v>6</v>
+      </c>
+      <c r="C293" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D293" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E293" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="F293" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A294" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B294" s="11">
+        <v>6</v>
+      </c>
+      <c r="C294" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="D294" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E294" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="F294" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A295" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B295" s="11">
+        <v>6</v>
+      </c>
+      <c r="C295" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="D295" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E295" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="F295" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A296" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B296" s="11">
+        <v>6</v>
+      </c>
+      <c r="C296" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D296" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E261" s="1" t="s">
+      <c r="E296" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="F296" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A297" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B297" s="11">
+        <v>6</v>
+      </c>
+      <c r="C297" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D297" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E297" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="F297" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A298" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B298" s="11">
+        <v>6</v>
+      </c>
+      <c r="C298" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D298" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E298" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="F298" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A299" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B299" s="11">
+        <v>6</v>
+      </c>
+      <c r="C299" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D299" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E299" s="12" t="s">
         <v>303</v>
       </c>
-      <c r="F261" s="1" t="s">
+      <c r="F299" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A300" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B300" s="11">
+        <v>6</v>
+      </c>
+      <c r="C300" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="D300" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E300" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="F300" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A301" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B301" s="11">
+        <v>6</v>
+      </c>
+      <c r="C301" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="D301" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E301" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="F301" s="1" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix US fonts and size
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Chain-of-Thought dataset/CoTDataset.xlsx
+++ b/refair-server/datasets/Chain-of-Thought dataset/CoTDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\Chain-of-Thought dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2C1A04-0EF8-4A2A-AE21-25A87613491A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB37C656-4BA3-4DF8-8714-8E7EF160B5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -1664,8 +1664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
   <dimension ref="A1:F341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A315" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C340" sqref="C340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -8464,7 +8464,7 @@
       <c r="B340" s="15">
         <v>6</v>
       </c>
-      <c r="C340" s="15" t="s">
+      <c r="C340" s="11" t="s">
         <v>345</v>
       </c>
       <c r="D340" s="2" t="s">
@@ -8484,7 +8484,7 @@
       <c r="B341" s="15">
         <v>6</v>
       </c>
-      <c r="C341" s="15" t="s">
+      <c r="C341" s="11" t="s">
         <v>347</v>
       </c>
       <c r="D341" s="2" t="s">

</xml_diff>

<commit_message>
Add US related to "Movies" and "Music" domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Chain-of-Thought dataset/CoTDataset.xlsx
+++ b/refair-server/datasets/Chain-of-Thought dataset/CoTDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\Chain-of-Thought Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F034C20-88B5-4579-9797-275CE54DE4B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3A2209-FCD1-443A-AEC3-ACD31C0DB229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2906" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3106" uniqueCount="685">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -1962,6 +1962,135 @@
   </si>
   <si>
     <t>As an urban sustainability analyst, I need to apply word embedding techniques to analyze textual data from urban sustainability reports and identify key sustainability concepts and trends, informing sustainable urban development strategies.</t>
+  </si>
+  <si>
+    <t>Sport &amp; Enterteinment</t>
+  </si>
+  <si>
+    <t>Movies</t>
+  </si>
+  <si>
+    <t>As a movie studio executive, I want to employ adversarial learning techniques to detect deepfake videos that maliciously use our actors' likenesses, so that we can protect our brand and actors' reputations.</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>As a music data scientist, I want to apply adversarial learning techniques to enhance the robustness of my music genre classification model, ensuring it accurately identifies genre boundaries even in the presence of adversarial attacks.</t>
+  </si>
+  <si>
+    <t>As a visual effects supervisor, I aim to use CNNs to automate the process of identifying and correcting green screen errors in movie footage, reducing production time and costs.</t>
+  </si>
+  <si>
+    <t>As a music audio engineer, I aim to utilize CNNs to develop a real-time music event detection system that can identify and timestamp specific musical events (e.g., beats, notes, transitions) in audio recordings.</t>
+  </si>
+  <si>
+    <t>As a casual moviegoer, I want a conversational agent to provide summaries and reviews for new movie releases, so that I can decide which films to watch next.</t>
+  </si>
+  <si>
+    <t>As a musician, I need a conversational AI assistant that can analyze my compositions using machine learning techniques, providing constructive feedback on musical structure, harmony, and creativity.</t>
+  </si>
+  <si>
+    <t>As a movie studio executive, I want to employ decision trees to predict the financial success of a movie based on its genre, director, and release date, so that I can make informed greenlighting decisions.</t>
+  </si>
+  <si>
+    <t>As a music event organizer, I need a decision tree-based system that recommends suitable artists and bands for events based on their musical style, popularity, and audience preferences extracted from past event data.</t>
+  </si>
+  <si>
+    <t>s a streaming platform administrator, I want to employ document classification to classify user-generated movie summaries into predefined genres (e.g., action, comedy, drama) automatically, so that I can enhance movie recommendation algorithms.</t>
+  </si>
+  <si>
+    <t>As a music journalist, I need a document classification system to organize news articles and reviews into topics like album releases, artist interviews, and concert reviews, making it easier to access and reference past work.</t>
+  </si>
+  <si>
+    <t>As a movie metadata curator, I want to develop an entity extraction system to automatically identify and extract key entities such as movie titles, directors, actors, and release dates from unstructured movie reviews and articles, so that I can maintain an up-to-date and accurate movie database.</t>
+  </si>
+  <si>
+    <t>As a music copyright manager, I aim to employ entity extraction to detect and flag copyrighted content in user-uploaded lyrics and compositions, ensuring compliance with intellectual property laws.</t>
+  </si>
+  <si>
+    <t>As a movie critic, I want to perform feature selection to identify the most influential factors (such as genre, director reputation, and cast popularity) that contribute to a movie's box office success, so that I can provide deeper insights into what makes a movie commercially appealing.</t>
+  </si>
+  <si>
+    <t>As a music content curator, I want to use feature selection to automate the process of identifying distinctive musical characteristics (e.g., instrumentation, vocal style) that define niche subgenres, facilitating targeted content curation for diverse listener preferences.</t>
+  </si>
+  <si>
+    <t>As a researcher studying movie box office performance, I want to handle class imbalance in datasets categorizing movies into blockbuster and non-blockbuster categories, so that I can develop predictive models that accurately forecast commercial success.</t>
+  </si>
+  <si>
+    <t>As a music recommendation system engineer, I aim to mitigate the impact of imbalanced data by employing techniques that prioritize user feedback on less popular songs, enhancing the diversity and fairness of music recommendations.</t>
+  </si>
+  <si>
+    <t>As a movie critic, I want to develop a keyword extraction system to automatically identify and extract key themes and topics from movie reviews, so that I can categorize and analyze critical opinions effectively.</t>
+  </si>
+  <si>
+    <t>As a music content curator, I need a keyword extraction tool that utilizes machine learning to automatically identify prominent themes and topics from music reviews and interviews, aiding in the creation of focused artist profiles and music playlists.</t>
+  </si>
+  <si>
+    <t>As a movie critic, I want to leverage KNN to identify movies with similar stylistic traits and narrative structures, so that I can analyze trends in filmmaking techniques and storytelling approaches over time.</t>
+  </si>
+  <si>
+    <t>As a music event organizer, I want to use a k-NN model to recommend suitable opening acts for headline artists based on their musical styles and fan demographics, ensuring cohesive and engaging concert lineups.</t>
+  </si>
+  <si>
+    <t>As a movie content moderator, I want to implement multi-label classification to automatically flag movies with appropriate content warnings (such as violence, nudity, and language) based on scene analysis and dialogue, so that I can ensure viewer suitability.</t>
+  </si>
+  <si>
+    <t>As a music recommendation system developer, I aim to build a multi-label classification model that can accurately tag songs with multiple genres (e.g., rock, pop, indie) based on their audio features and lyrical content, enhancing the diversity and relevance of music recommendations.</t>
+  </si>
+  <si>
+    <t>As a special effects supervisor, I want to develop a neural network model to simulate realistic visual effects (such as explosions and CGI creatures) in movies based on physical parameters and environmental conditions, so that I can achieve cinematic realism.</t>
+  </si>
+  <si>
+    <t>As a music audio quality evaluator, I want to develop a neural network model that assesses the audio quality of music recordings by analyzing various audio features such as clarity, dynamic range, and noise levels, ensuring high fidelity in music production and distribution.</t>
+  </si>
+  <si>
+    <t>As a movie critic, I want to build a random forest model to predict movie box office success based on features such as genre, cast popularity, and promotional budget, so that I can analyze factors contributing to financial performance.</t>
+  </si>
+  <si>
+    <t>As a music content curator, I seek to utilize a random forest model to automatically classify newly released songs into thematic categories (e.g., party music, workout tunes, relaxing melodies) based on their audio attributes, facilitating targeted playlist curation and content discovery.</t>
+  </si>
+  <si>
+    <t>As a movie review aggregator, I want to develop a semantic similarity model to identify and group similar movie reviews based on their thematic content and sentiment, so that I can summarize overall audience reactions more effectively.</t>
+  </si>
+  <si>
+    <t>As a music content aggregator, I seek to employ semantic similarity algorithms to cluster music news articles and reviews based on shared topics, enabling efficient content aggregation and providing comprehensive coverage of trending music topics.</t>
+  </si>
+  <si>
+    <t>As a movie critic, I want to develop a sentiment analysis model to automatically classify movie reviews as positive, neutral, or negative based on textual content, so that I can gauge overall audience sentiment towards a movie.</t>
+  </si>
+  <si>
+    <t>As a music marketing strategist, I want to use sentiment analysis to monitor social media sentiment around new music releases and artist announcements, gauging public reception and adjusting marketing campaigns accordingly.</t>
+  </si>
+  <si>
+    <t>As a movie review aggregator, I want to implement speech-to-text technology to transcribe audiovisual movie reviews from podcasts and video reviews into text format, so that I can include diverse content sources in my review summaries.</t>
+  </si>
+  <si>
+    <t>As a music journalist, I seek to use speech-to-text tools to transcribe artist interviews and press conferences efficiently, enabling quicker turnaround for articles and features covering music industry news and events.</t>
+  </si>
+  <si>
+    <t>s a movie script analyst, I want to employ text categorization to classify movie scripts into different narrative styles and thematic categories (e.g., romance, action-adventure, science fiction), so that I can analyze storytelling trends and genre preferences over time.</t>
+  </si>
+  <si>
+    <t>As a music content curator, I need a text categorization model to automatically categorize music reviews and critiques into genres (e.g., rock, jazz, classical) based on textual content, facilitating efficient content tagging and organization.</t>
+  </si>
+  <si>
+    <t>As a movie critic, I want to utilize unsupervised clustering to group movies into clusters based on thematic elements and directorial styles, so that I can explore connections between movies and provide insightful reviews on thematic similarities.</t>
+  </si>
+  <si>
+    <t>As a music playlist curator, I seek to use unsupervised clustering techniques to cluster user-generated playlists into groups based on similarity in musical styles, facilitating the discovery of new playlist ideas and enhancing playlist diversity.</t>
+  </si>
+  <si>
+    <t>As a movie subtitle creator, I want to develop a voice recognition system to accurately transcribe movie dialogues from audio tracks into text, so that I can create synchronized subtitles for hearing-impaired viewers.</t>
+  </si>
+  <si>
+    <t>As a music event organizer, I aim to utilize voice recognition technology for real-time transcription of panel discussions, workshops, and keynote speeches at music conferences and industry events, facilitating knowledge sharing and accessibility for attendees.</t>
+  </si>
+  <si>
+    <t>As a movie content curator, I want to use word embedding techniques to analyze similarities and relationships between movie plot summaries based on semantic meanings of key words and phrases, so that I can categorize and recommend related movies effectively.</t>
+  </si>
+  <si>
+    <t>As a music content curator, I seek to employ word embedding algorithms to analyze and categorize music-related textual content (e.g., artist bios, album reviews) based on underlying semantic similarities, facilitating more intuitive content organization and retrieval.</t>
   </si>
 </sst>
 </file>
@@ -2012,25 +2141,29 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2085,6 +2218,12 @@
         <bgColor rgb="FFD9D2E9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA2C4C9"/>
+        <bgColor rgb="FFA2C4C9"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -2114,7 +2253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2157,6 +2296,7 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2492,10 +2632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F581"/>
+  <dimension ref="A1:F621"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A555" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F421" sqref="F421:F581"/>
+    <sheetView tabSelected="1" topLeftCell="A598" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F581" sqref="F581:F621"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -14127,6 +14267,806 @@
         <v>49</v>
       </c>
     </row>
+    <row r="582" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A582" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B582" s="22">
+        <v>8</v>
+      </c>
+      <c r="C582" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D582" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E582" t="s">
+        <v>644</v>
+      </c>
+      <c r="F582" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="583" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A583" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B583" s="22">
+        <v>8</v>
+      </c>
+      <c r="C583" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D583" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E583" t="s">
+        <v>646</v>
+      </c>
+      <c r="F583" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="584" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A584" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B584" s="22">
+        <v>8</v>
+      </c>
+      <c r="C584" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D584" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E584" t="s">
+        <v>647</v>
+      </c>
+      <c r="F584" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="585" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A585" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B585" s="22">
+        <v>8</v>
+      </c>
+      <c r="C585" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D585" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E585" t="s">
+        <v>648</v>
+      </c>
+      <c r="F585" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="586" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A586" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B586" s="22">
+        <v>8</v>
+      </c>
+      <c r="C586" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D586" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E586" t="s">
+        <v>649</v>
+      </c>
+      <c r="F586" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="587" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A587" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B587" s="22">
+        <v>8</v>
+      </c>
+      <c r="C587" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D587" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E587" t="s">
+        <v>650</v>
+      </c>
+      <c r="F587" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="588" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A588" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B588" s="22">
+        <v>8</v>
+      </c>
+      <c r="C588" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D588" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E588" t="s">
+        <v>651</v>
+      </c>
+      <c r="F588" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="589" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A589" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B589" s="22">
+        <v>8</v>
+      </c>
+      <c r="C589" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D589" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E589" t="s">
+        <v>652</v>
+      </c>
+      <c r="F589" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="590" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A590" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B590" s="22">
+        <v>8</v>
+      </c>
+      <c r="C590" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D590" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E590" t="s">
+        <v>653</v>
+      </c>
+      <c r="F590" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="591" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A591" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B591" s="22">
+        <v>8</v>
+      </c>
+      <c r="C591" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D591" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E591" t="s">
+        <v>654</v>
+      </c>
+      <c r="F591" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="592" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A592" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B592" s="22">
+        <v>8</v>
+      </c>
+      <c r="C592" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D592" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E592" t="s">
+        <v>655</v>
+      </c>
+      <c r="F592" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="593" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A593" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B593" s="22">
+        <v>8</v>
+      </c>
+      <c r="C593" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D593" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E593" t="s">
+        <v>656</v>
+      </c>
+      <c r="F593" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="594" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A594" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B594" s="22">
+        <v>8</v>
+      </c>
+      <c r="C594" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D594" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E594" t="s">
+        <v>657</v>
+      </c>
+      <c r="F594" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="595" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A595" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B595" s="22">
+        <v>8</v>
+      </c>
+      <c r="C595" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D595" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E595" t="s">
+        <v>658</v>
+      </c>
+      <c r="F595" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="596" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A596" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B596" s="22">
+        <v>8</v>
+      </c>
+      <c r="C596" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D596" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E596" t="s">
+        <v>659</v>
+      </c>
+      <c r="F596" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="597" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A597" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B597" s="22">
+        <v>8</v>
+      </c>
+      <c r="C597" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D597" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E597" t="s">
+        <v>660</v>
+      </c>
+      <c r="F597" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="598" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A598" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B598" s="22">
+        <v>8</v>
+      </c>
+      <c r="C598" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D598" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E598" t="s">
+        <v>661</v>
+      </c>
+      <c r="F598" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="599" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A599" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B599" s="22">
+        <v>8</v>
+      </c>
+      <c r="C599" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D599" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E599" t="s">
+        <v>662</v>
+      </c>
+      <c r="F599" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="600" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A600" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B600" s="22">
+        <v>8</v>
+      </c>
+      <c r="C600" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D600" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E600" t="s">
+        <v>663</v>
+      </c>
+      <c r="F600" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="601" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A601" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B601" s="22">
+        <v>8</v>
+      </c>
+      <c r="C601" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D601" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E601" t="s">
+        <v>664</v>
+      </c>
+      <c r="F601" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="602" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A602" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B602" s="22">
+        <v>8</v>
+      </c>
+      <c r="C602" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D602" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E602" t="s">
+        <v>665</v>
+      </c>
+      <c r="F602" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="603" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A603" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B603" s="22">
+        <v>8</v>
+      </c>
+      <c r="C603" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D603" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E603" t="s">
+        <v>666</v>
+      </c>
+      <c r="F603" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="604" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A604" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B604" s="22">
+        <v>8</v>
+      </c>
+      <c r="C604" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D604" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E604" t="s">
+        <v>667</v>
+      </c>
+      <c r="F604" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="605" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A605" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B605" s="22">
+        <v>8</v>
+      </c>
+      <c r="C605" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D605" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E605" t="s">
+        <v>668</v>
+      </c>
+      <c r="F605" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="606" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A606" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B606" s="22">
+        <v>8</v>
+      </c>
+      <c r="C606" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D606" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E606" t="s">
+        <v>669</v>
+      </c>
+      <c r="F606" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="607" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A607" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B607" s="22">
+        <v>8</v>
+      </c>
+      <c r="C607" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D607" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E607" t="s">
+        <v>670</v>
+      </c>
+      <c r="F607" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="608" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A608" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B608" s="22">
+        <v>8</v>
+      </c>
+      <c r="C608" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D608" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E608" t="s">
+        <v>671</v>
+      </c>
+      <c r="F608" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="609" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A609" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B609" s="22">
+        <v>8</v>
+      </c>
+      <c r="C609" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D609" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E609" t="s">
+        <v>672</v>
+      </c>
+      <c r="F609" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="610" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A610" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B610" s="22">
+        <v>8</v>
+      </c>
+      <c r="C610" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D610" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E610" t="s">
+        <v>673</v>
+      </c>
+      <c r="F610" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="611" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A611" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B611" s="22">
+        <v>8</v>
+      </c>
+      <c r="C611" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D611" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E611" t="s">
+        <v>674</v>
+      </c>
+      <c r="F611" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="612" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A612" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B612" s="22">
+        <v>8</v>
+      </c>
+      <c r="C612" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D612" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E612" t="s">
+        <v>675</v>
+      </c>
+      <c r="F612" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="613" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A613" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B613" s="22">
+        <v>8</v>
+      </c>
+      <c r="C613" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D613" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E613" t="s">
+        <v>676</v>
+      </c>
+      <c r="F613" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="614" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A614" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B614" s="22">
+        <v>8</v>
+      </c>
+      <c r="C614" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D614" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E614" t="s">
+        <v>677</v>
+      </c>
+      <c r="F614" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="615" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A615" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B615" s="22">
+        <v>8</v>
+      </c>
+      <c r="C615" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D615" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E615" t="s">
+        <v>678</v>
+      </c>
+      <c r="F615" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="616" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A616" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B616" s="22">
+        <v>8</v>
+      </c>
+      <c r="C616" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D616" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E616" t="s">
+        <v>679</v>
+      </c>
+      <c r="F616" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="617" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A617" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B617" s="22">
+        <v>8</v>
+      </c>
+      <c r="C617" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D617" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E617" t="s">
+        <v>680</v>
+      </c>
+      <c r="F617" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="618" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A618" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B618" s="22">
+        <v>8</v>
+      </c>
+      <c r="C618" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D618" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E618" t="s">
+        <v>681</v>
+      </c>
+      <c r="F618" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="619" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A619" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B619" s="22">
+        <v>8</v>
+      </c>
+      <c r="C619" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D619" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E619" t="s">
+        <v>682</v>
+      </c>
+      <c r="F619" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="620" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A620" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B620" s="22">
+        <v>8</v>
+      </c>
+      <c r="C620" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D620" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E620" t="s">
+        <v>683</v>
+      </c>
+      <c r="F620" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="621" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A621" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B621" s="22">
+        <v>8</v>
+      </c>
+      <c r="C621" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D621" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E621" t="s">
+        <v>684</v>
+      </c>
+      <c r="F621" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A162:F221">
     <sortCondition ref="D1:D221"/>

</xml_diff>

<commit_message>
Add US related to "Sport"  domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Chain-of-Thought dataset/CoTDataset.xlsx
+++ b/refair-server/datasets/Chain-of-Thought dataset/CoTDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\Chain-of-Thought Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3A2209-FCD1-443A-AEC3-ACD31C0DB229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B101E874-343B-42AE-9332-D93850FFFA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3106" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3206" uniqueCount="706">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -2091,6 +2091,69 @@
   </si>
   <si>
     <t>As a music content curator, I seek to employ word embedding algorithms to analyze and categorize music-related textual content (e.g., artist bios, album reviews) based on underlying semantic similarities, facilitating more intuitive content organization and retrieval.</t>
+  </si>
+  <si>
+    <t>Sport</t>
+  </si>
+  <si>
+    <t>As a coach, I want to utilize adversarial learning models to simulate opponents' strategies and tactics based on historical data, in order to better prepare my team for upcoming matches.</t>
+  </si>
+  <si>
+    <t>As a sports video analyst, I want to use CNNs to automatically track and analyze player movements during games, providing coaches with detailed insights into player positioning and performance metrics.</t>
+  </si>
+  <si>
+    <t>As a sports team manager, I want to develop a conversational agent powered by machine learning to provide real-time updates on player injuries, performance statistics, and training schedules, enhancing communication and coordination within the team.</t>
+  </si>
+  <si>
+    <t>As a sports physiologist, I want to employ a decision tree algorithm to classify and diagnose common sports injuries based on symptoms, patient history, and diagnostic tests, aiding in timely and accurate treatment plans.</t>
+  </si>
+  <si>
+    <t>As a sports journalist, I want to develop a document classification model to automatically categorize news articles into relevant sports categories such as football, basketball, and tennis, facilitating quicker content retrieval and publication.</t>
+  </si>
+  <si>
+    <t>As a sports betting analyst, I want to develop an entity extraction model to extract key statistics such as player performance metrics, injury updates, and historical match results from sports betting websites and databases, facilitating data-driven betting strategies.</t>
+  </si>
+  <si>
+    <t>As a sports performance analyst, I want to employ feature selection techniques to identify the most relevant player performance metrics (such as goals scored, assists, and accuracy) that correlate with team success, aiding in player evaluation and strategy formulation.</t>
+  </si>
+  <si>
+    <t>As a sports talent scout, I want to build a recruitment model that handles imbalanced data by accurately identifying and prioritizing promising young athletes from underrepresented regions or sports disciplines, ensuring comprehensive talent evaluation</t>
+  </si>
+  <si>
+    <t>As a sports content curator, I want to implement keyword extraction techniques to analyze player interviews and press conferences, automatically extracting key themes and quotes for creating engaging multimedia content for fans.</t>
+  </si>
+  <si>
+    <t>As a sports talent scout, I want to use k-NN clustering to group young athletes based on their physical attributes, skill levels, and potential for development, facilitating more targeted scouting and recruitment efforts.</t>
+  </si>
+  <si>
+    <t>As a sports physiologist, I want to develop a multi-label classification model to predict the physiological responses (such as heart rate, oxygen consumption) of athletes during different phases of a game or training session, based on various environmental and physical factors.</t>
+  </si>
+  <si>
+    <t>As a sports video analyst, I want to develop a convolutional neural network (CNN) to automatically analyze player movements and positions from video footage, extracting tactical insights and performance metrics for coaching and strategy refinement.</t>
+  </si>
+  <si>
+    <t>As a sports betting strategist, I want to build a random forest model to predict betting odds for various outcomes in sports matches, considering factors such as team form, player statistics, and historical match data, to inform strategic betting decisions.</t>
+  </si>
+  <si>
+    <t>As a sports content curator, I want to develop a semantic similarity model to recommend relevant articles, videos, and social media posts to fans based on their interests and engagement history, enhancing personalized content delivery.</t>
+  </si>
+  <si>
+    <t>As a sports broadcaster, I want to develop a sentiment analysis model to analyze viewer reactions and sentiment towards live sports broadcasts, helping us understand audience engagement and preferences.</t>
+  </si>
+  <si>
+    <t>As a sports journalist, I want to leverage speech-to-text technology to transcribe interviews with athletes and coaches, enabling faster content creation and accurate reporting of quotes and insights.</t>
+  </si>
+  <si>
+    <t>As a sports news aggregator, I want to develop a text categorization model to classify news articles into different sports categories such as football, basketball, tennis, etc., ensuring relevant and organized content delivery to users.</t>
+  </si>
+  <si>
+    <t>As a sports scouting coordinator, I want to use unsupervised clustering techniques to cluster and analyze player statistics and attributes to identify emerging talents and potential recruits, streamlining talent scouting and recruitment processes.</t>
+  </si>
+  <si>
+    <t>As a sports broadcaster, I want to deploy voice recognition systems to automatically generate transcripts of sports podcasts and radio shows, enabling searchable archives and content summaries for listeners.</t>
+  </si>
+  <si>
+    <t>As a sports content curator, I want to apply word embedding models to recommend related articles and videos to sports fans based on semantic similarities in content, enhancing user engagement and content discovery.</t>
   </si>
 </sst>
 </file>
@@ -2632,10 +2695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F621"/>
+  <dimension ref="A1:F641"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A598" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F581" sqref="F581:F621"/>
+    <sheetView tabSelected="1" topLeftCell="A621" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F621" sqref="F621:F641"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -14315,13 +14378,13 @@
         <v>8</v>
       </c>
       <c r="C584" s="22" t="s">
-        <v>643</v>
+        <v>685</v>
       </c>
       <c r="D584" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E584" t="s">
-        <v>647</v>
+        <v>686</v>
       </c>
       <c r="F584" s="1" t="s">
         <v>49</v>
@@ -14335,13 +14398,13 @@
         <v>8</v>
       </c>
       <c r="C585" s="22" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D585" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E585" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F585" s="1" t="s">
         <v>49</v>
@@ -14355,13 +14418,13 @@
         <v>8</v>
       </c>
       <c r="C586" s="22" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D586" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E586" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="F586" s="1" t="s">
         <v>49</v>
@@ -14375,13 +14438,13 @@
         <v>8</v>
       </c>
       <c r="C587" s="22" t="s">
-        <v>645</v>
+        <v>685</v>
       </c>
       <c r="D587" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E587" t="s">
-        <v>650</v>
+        <v>687</v>
       </c>
       <c r="F587" s="1" t="s">
         <v>49</v>
@@ -14398,10 +14461,10 @@
         <v>643</v>
       </c>
       <c r="D588" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E588" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="F588" s="1" t="s">
         <v>49</v>
@@ -14418,10 +14481,10 @@
         <v>645</v>
       </c>
       <c r="D589" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E589" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="F589" s="1" t="s">
         <v>49</v>
@@ -14435,13 +14498,13 @@
         <v>8</v>
       </c>
       <c r="C590" s="22" t="s">
-        <v>643</v>
+        <v>685</v>
       </c>
       <c r="D590" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E590" t="s">
-        <v>653</v>
+        <v>688</v>
       </c>
       <c r="F590" s="1" t="s">
         <v>49</v>
@@ -14455,13 +14518,13 @@
         <v>8</v>
       </c>
       <c r="C591" s="22" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D591" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E591" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="F591" s="1" t="s">
         <v>49</v>
@@ -14475,13 +14538,13 @@
         <v>8</v>
       </c>
       <c r="C592" s="22" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D592" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E592" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="F592" s="1" t="s">
         <v>49</v>
@@ -14495,13 +14558,13 @@
         <v>8</v>
       </c>
       <c r="C593" s="22" t="s">
-        <v>645</v>
+        <v>685</v>
       </c>
       <c r="D593" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E593" t="s">
-        <v>656</v>
+        <v>689</v>
       </c>
       <c r="F593" s="1" t="s">
         <v>49</v>
@@ -14518,10 +14581,10 @@
         <v>643</v>
       </c>
       <c r="D594" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E594" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="F594" s="1" t="s">
         <v>49</v>
@@ -14538,10 +14601,10 @@
         <v>645</v>
       </c>
       <c r="D595" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E595" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="F595" s="1" t="s">
         <v>49</v>
@@ -14555,13 +14618,13 @@
         <v>8</v>
       </c>
       <c r="C596" s="22" t="s">
-        <v>643</v>
+        <v>685</v>
       </c>
       <c r="D596" s="2" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E596" t="s">
-        <v>659</v>
+        <v>690</v>
       </c>
       <c r="F596" s="1" t="s">
         <v>49</v>
@@ -14575,13 +14638,13 @@
         <v>8</v>
       </c>
       <c r="C597" s="22" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D597" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E597" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="F597" s="1" t="s">
         <v>49</v>
@@ -14595,13 +14658,13 @@
         <v>8</v>
       </c>
       <c r="C598" s="22" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D598" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E598" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="F598" s="1" t="s">
         <v>49</v>
@@ -14615,13 +14678,13 @@
         <v>8</v>
       </c>
       <c r="C599" s="22" t="s">
-        <v>645</v>
+        <v>685</v>
       </c>
       <c r="D599" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E599" t="s">
-        <v>662</v>
+        <v>691</v>
       </c>
       <c r="F599" s="1" t="s">
         <v>49</v>
@@ -14638,10 +14701,10 @@
         <v>643</v>
       </c>
       <c r="D600" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E600" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="F600" s="1" t="s">
         <v>49</v>
@@ -14658,10 +14721,10 @@
         <v>645</v>
       </c>
       <c r="D601" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E601" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="F601" s="1" t="s">
         <v>49</v>
@@ -14675,13 +14738,13 @@
         <v>8</v>
       </c>
       <c r="C602" s="22" t="s">
-        <v>643</v>
+        <v>685</v>
       </c>
       <c r="D602" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E602" t="s">
-        <v>665</v>
+        <v>692</v>
       </c>
       <c r="F602" s="1" t="s">
         <v>49</v>
@@ -14695,13 +14758,13 @@
         <v>8</v>
       </c>
       <c r="C603" s="22" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D603" s="2" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E603" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
       <c r="F603" s="1" t="s">
         <v>49</v>
@@ -14715,13 +14778,13 @@
         <v>8</v>
       </c>
       <c r="C604" s="22" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D604" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E604" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
       <c r="F604" s="1" t="s">
         <v>49</v>
@@ -14735,13 +14798,13 @@
         <v>8</v>
       </c>
       <c r="C605" s="22" t="s">
-        <v>645</v>
+        <v>685</v>
       </c>
       <c r="D605" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E605" t="s">
-        <v>668</v>
+        <v>693</v>
       </c>
       <c r="F605" s="1" t="s">
         <v>49</v>
@@ -14758,10 +14821,10 @@
         <v>643</v>
       </c>
       <c r="D606" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E606" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
       <c r="F606" s="1" t="s">
         <v>49</v>
@@ -14778,10 +14841,10 @@
         <v>645</v>
       </c>
       <c r="D607" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E607" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="F607" s="1" t="s">
         <v>49</v>
@@ -14795,13 +14858,13 @@
         <v>8</v>
       </c>
       <c r="C608" s="22" t="s">
-        <v>643</v>
+        <v>685</v>
       </c>
       <c r="D608" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E608" t="s">
-        <v>671</v>
+        <v>694</v>
       </c>
       <c r="F608" s="1" t="s">
         <v>49</v>
@@ -14815,13 +14878,13 @@
         <v>8</v>
       </c>
       <c r="C609" s="22" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D609" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E609" t="s">
-        <v>672</v>
+        <v>663</v>
       </c>
       <c r="F609" s="1" t="s">
         <v>49</v>
@@ -14835,13 +14898,13 @@
         <v>8</v>
       </c>
       <c r="C610" s="22" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D610" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E610" t="s">
-        <v>673</v>
+        <v>664</v>
       </c>
       <c r="F610" s="1" t="s">
         <v>49</v>
@@ -14855,13 +14918,13 @@
         <v>8</v>
       </c>
       <c r="C611" s="22" t="s">
-        <v>645</v>
+        <v>685</v>
       </c>
       <c r="D611" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E611" t="s">
-        <v>674</v>
+        <v>695</v>
       </c>
       <c r="F611" s="1" t="s">
         <v>49</v>
@@ -14878,10 +14941,10 @@
         <v>643</v>
       </c>
       <c r="D612" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E612" t="s">
-        <v>675</v>
+        <v>665</v>
       </c>
       <c r="F612" s="1" t="s">
         <v>49</v>
@@ -14898,10 +14961,10 @@
         <v>645</v>
       </c>
       <c r="D613" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E613" t="s">
-        <v>676</v>
+        <v>666</v>
       </c>
       <c r="F613" s="1" t="s">
         <v>49</v>
@@ -14915,13 +14978,13 @@
         <v>8</v>
       </c>
       <c r="C614" s="22" t="s">
-        <v>643</v>
+        <v>685</v>
       </c>
       <c r="D614" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E614" t="s">
-        <v>677</v>
+        <v>696</v>
       </c>
       <c r="F614" s="1" t="s">
         <v>49</v>
@@ -14935,13 +14998,13 @@
         <v>8</v>
       </c>
       <c r="C615" s="22" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D615" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E615" t="s">
-        <v>678</v>
+        <v>667</v>
       </c>
       <c r="F615" s="1" t="s">
         <v>49</v>
@@ -14955,13 +15018,13 @@
         <v>8</v>
       </c>
       <c r="C616" s="22" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D616" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E616" t="s">
-        <v>679</v>
+        <v>668</v>
       </c>
       <c r="F616" s="1" t="s">
         <v>49</v>
@@ -14975,13 +15038,13 @@
         <v>8</v>
       </c>
       <c r="C617" s="22" t="s">
-        <v>645</v>
+        <v>685</v>
       </c>
       <c r="D617" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E617" t="s">
-        <v>680</v>
+        <v>697</v>
       </c>
       <c r="F617" s="1" t="s">
         <v>49</v>
@@ -14998,10 +15061,10 @@
         <v>643</v>
       </c>
       <c r="D618" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E618" t="s">
-        <v>681</v>
+        <v>669</v>
       </c>
       <c r="F618" s="1" t="s">
         <v>49</v>
@@ -15018,10 +15081,10 @@
         <v>645</v>
       </c>
       <c r="D619" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E619" t="s">
-        <v>682</v>
+        <v>670</v>
       </c>
       <c r="F619" s="1" t="s">
         <v>49</v>
@@ -15035,13 +15098,13 @@
         <v>8</v>
       </c>
       <c r="C620" s="22" t="s">
-        <v>643</v>
+        <v>685</v>
       </c>
       <c r="D620" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E620" t="s">
-        <v>683</v>
+        <v>698</v>
       </c>
       <c r="F620" s="1" t="s">
         <v>49</v>
@@ -15055,15 +15118,415 @@
         <v>8</v>
       </c>
       <c r="C621" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D621" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E621" t="s">
+        <v>671</v>
+      </c>
+      <c r="F621" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="622" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A622" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B622" s="22">
+        <v>8</v>
+      </c>
+      <c r="C622" s="22" t="s">
         <v>645</v>
       </c>
-      <c r="D621" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E621" t="s">
+      <c r="D622" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E622" t="s">
+        <v>672</v>
+      </c>
+      <c r="F622" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="623" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A623" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B623" s="22">
+        <v>8</v>
+      </c>
+      <c r="C623" s="22" t="s">
+        <v>685</v>
+      </c>
+      <c r="D623" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E623" t="s">
+        <v>699</v>
+      </c>
+      <c r="F623" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="624" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A624" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B624" s="22">
+        <v>8</v>
+      </c>
+      <c r="C624" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D624" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E624" t="s">
+        <v>673</v>
+      </c>
+      <c r="F624" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="625" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A625" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B625" s="22">
+        <v>8</v>
+      </c>
+      <c r="C625" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D625" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E625" t="s">
+        <v>674</v>
+      </c>
+      <c r="F625" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="626" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A626" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B626" s="22">
+        <v>8</v>
+      </c>
+      <c r="C626" s="22" t="s">
+        <v>685</v>
+      </c>
+      <c r="D626" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E626" t="s">
+        <v>700</v>
+      </c>
+      <c r="F626" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="627" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A627" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B627" s="22">
+        <v>8</v>
+      </c>
+      <c r="C627" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D627" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E627" t="s">
+        <v>675</v>
+      </c>
+      <c r="F627" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="628" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A628" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B628" s="22">
+        <v>8</v>
+      </c>
+      <c r="C628" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D628" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E628" t="s">
+        <v>676</v>
+      </c>
+      <c r="F628" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="629" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A629" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B629" s="22">
+        <v>8</v>
+      </c>
+      <c r="C629" s="22" t="s">
+        <v>685</v>
+      </c>
+      <c r="D629" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E629" t="s">
+        <v>701</v>
+      </c>
+      <c r="F629" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="630" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A630" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B630" s="22">
+        <v>8</v>
+      </c>
+      <c r="C630" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D630" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E630" t="s">
+        <v>677</v>
+      </c>
+      <c r="F630" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="631" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A631" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B631" s="22">
+        <v>8</v>
+      </c>
+      <c r="C631" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D631" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E631" t="s">
+        <v>678</v>
+      </c>
+      <c r="F631" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="632" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A632" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B632" s="22">
+        <v>8</v>
+      </c>
+      <c r="C632" s="22" t="s">
+        <v>685</v>
+      </c>
+      <c r="D632" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E632" t="s">
+        <v>702</v>
+      </c>
+      <c r="F632" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="633" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A633" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B633" s="22">
+        <v>8</v>
+      </c>
+      <c r="C633" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D633" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E633" t="s">
+        <v>679</v>
+      </c>
+      <c r="F633" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="634" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A634" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B634" s="22">
+        <v>8</v>
+      </c>
+      <c r="C634" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D634" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E634" t="s">
+        <v>680</v>
+      </c>
+      <c r="F634" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="635" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A635" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B635" s="22">
+        <v>8</v>
+      </c>
+      <c r="C635" s="22" t="s">
+        <v>685</v>
+      </c>
+      <c r="D635" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E635" t="s">
+        <v>703</v>
+      </c>
+      <c r="F635" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="636" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A636" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B636" s="22">
+        <v>8</v>
+      </c>
+      <c r="C636" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D636" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E636" t="s">
+        <v>681</v>
+      </c>
+      <c r="F636" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="637" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A637" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B637" s="22">
+        <v>8</v>
+      </c>
+      <c r="C637" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D637" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E637" t="s">
+        <v>682</v>
+      </c>
+      <c r="F637" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="638" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A638" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B638" s="22">
+        <v>8</v>
+      </c>
+      <c r="C638" s="22" t="s">
+        <v>685</v>
+      </c>
+      <c r="D638" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E638" t="s">
+        <v>704</v>
+      </c>
+      <c r="F638" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="639" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A639" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B639" s="22">
+        <v>8</v>
+      </c>
+      <c r="C639" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D639" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E639" t="s">
+        <v>683</v>
+      </c>
+      <c r="F639" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="640" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A640" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B640" s="22">
+        <v>8</v>
+      </c>
+      <c r="C640" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="D640" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E640" t="s">
         <v>684</v>
       </c>
-      <c r="F621" s="1" t="s">
+      <c r="F640" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="641" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A641" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="B641" s="22">
+        <v>8</v>
+      </c>
+      <c r="C641" s="22" t="s">
+        <v>685</v>
+      </c>
+      <c r="D641" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E641" t="s">
+        <v>705</v>
+      </c>
+      <c r="F641" s="1" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add US related to Computer Networks" and "Computer Vision" domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Chain-of-Thought dataset/CoTDataset.xlsx
+++ b/refair-server/datasets/Chain-of-Thought dataset/CoTDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\Chain-of-Thought Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B101E874-343B-42AE-9332-D93850FFFA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C814A2DB-B3BF-41C3-8335-C9842E487D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3206" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3406" uniqueCount="749">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -2154,6 +2154,135 @@
   </si>
   <si>
     <t>As a sports content curator, I want to apply word embedding models to recommend related articles and videos to sports fans based on semantic similarities in content, enhancing user engagement and content discovery.</t>
+  </si>
+  <si>
+    <t>Technical Domains</t>
+  </si>
+  <si>
+    <t>Computer Networks</t>
+  </si>
+  <si>
+    <t>As a network intrusion detection specialist, I need to develop an adversarial learning model to enhance our system's ability to identify and classify sophisticated network intrusions in real-time.</t>
+  </si>
+  <si>
+    <t>Computer Vision</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to explore adversarial training techniques to improve the robustness of my image classification model against perturbations, so that it can maintain high accuracy even when presented with adversarial examples.</t>
+  </si>
+  <si>
+    <t>As a network performance engineer, I want to utilize CNNs to analyze network traffic patterns and identify bottlenecks in real-time, allowing for proactive optimization and resource allocation.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to explore transfer learning with CNNs for medical image analysis, so that a model trained on one type of medical imaging data (e.g., X-rays) can be adapted to analyze another type (e.g., MRIs) with minimal additional training.</t>
+  </si>
+  <si>
+    <t>As a network administrator, I need a conversational agent that can analyze network logs and provide real-time insights into performance metrics, helping me diagnose and resolve network congestion issues swiftly.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to develop a conversational agent that can answer questions about images, so that users can obtain information or descriptions of visual content through natural language interaction.</t>
+  </si>
+  <si>
+    <t>As a network capacity planner, I want to utilize decision tree analysis to forecast future bandwidth demands based on historical usage data, facilitating efficient resource allocation and scalability planning.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to employ decision trees for image segmentation in medical imaging applications, so that different tissues or anomalies within medical scans can be accurately delineated and analyzed.</t>
+  </si>
+  <si>
+    <t>As a network compliance officer, I want to implement document classification to classify network policies and procedures into relevant categories, ensuring adherence to regulatory standards.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to develop a document classification system that can automatically categorize scanned documents into predefined classes (e.g., invoices, contracts, reports), so that document management processes can be streamlined and organized.</t>
+  </si>
+  <si>
+    <t>As a network inventory manager, I aim to develop an entity extraction system to extract hardware component details (e.g., model numbers, serial numbers) from equipment inventory records, ensuring accurate asset management.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to implement entity extraction techniques for extracting product names, prices, and descriptions from e-commerce product catalogs, so that online retailers can maintain accurate inventory and pricing information.</t>
+  </si>
+  <si>
+    <t>As a network performance analyst, I need to perform feature selection to identify the most relevant metrics (e.g., latency, throughput) from network monitoring data for predicting congestion and optimizing traffic management.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to perform feature selection to identify the most discriminative visual features for object detection in images, so that the model can achieve high accuracy while reducing computational complexity.</t>
+  </si>
+  <si>
+    <t>As a network intrusion detection analyst, I need to address class imbalance in network attack datasets by applying sampling techniques (e.g., SMOTE, undersampling) to improve the performance of our anomaly detection models.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I need to address the challenge of imbalanced datasets in satellite image analysis by developing machine learning models capable of accurately identifying rare environmental anomalies for ecological monitoring.</t>
+  </si>
+  <si>
+    <t>As a network monitoring specialist, I aim to develop a system for real-time keyword extraction from network traffic logs to identify trends and patterns related to performance issues or potential security breaches.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to develop a keyword extraction model for automated image captioning, so that descriptive and relevant keywords can be generated to accompany images in applications like social media platforms or news articles.</t>
+  </si>
+  <si>
+    <t>As a network capacity planner, I aim to use k-NN regression to predict future network traffic patterns based on historical data, enabling proactive capacity scaling and resource allocation.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to implement k-Nearest Neighbor algorithm for image classification, so that I can create a baseline model to compare against more complex algorithms like CNNs (Convolutional Neural Networks).</t>
+  </si>
+  <si>
+    <t>As a network performance engineer, I want to develop a multi-label classification system to categorize network anomalies into different types (e.g., latency spikes, packet loss) for targeted troubleshooting and performance optimization.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to develop a multi-label classification model for autonomous vehicle perception, so that I can simultaneously detect and classify multiple objects such as pedestrians, vehicles, and traffic signs in real-time.</t>
+  </si>
+  <si>
+    <t>As a network reliability engineer, I want to utilize a neural network for predictive maintenance of network hardware by analyzing sensor data and predicting potential equipment failures before they occur, minimizing downtime.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to deploy a pre-trained deep learning model such as ResNet or VGG for feature extraction in content-based image retrieval systems, so that users can search and retrieve images based on visual similarity to a query image.</t>
+  </si>
+  <si>
+    <t>As a network security analyst, I need to deploy a random forest classifier to detect and classify various types of network intrusions and anomalies based on aggregated network traffic features, enhancing our cybersecurity defenses.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to utilize random forest-based anomaly detection techniques to identify unusual patterns or objects in security camera feeds, so that potential threats or abnormal activities can be detected in real-time.</t>
+  </si>
+  <si>
+    <t>As a network documentation manager, I aim to develop a semantic similarity algorithm to automatically identify redundant or overlapping information across network documentation, improving document organization and clarity.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to implement semantic similarity techniques to measure the similarity between scenes captured by different surveillance cameras, so that suspicious activities can be identified across multiple camera feeds in real-time.</t>
+  </si>
+  <si>
+    <t>As a network service provider, I need to perform sentiment analysis on customer feedback and support tickets related to network services to gauge customer satisfaction levels and identify areas for improvement.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to develop a sentiment analysis model for analyzing user emotions from facial expressions captured in real-time video feeds, so that the model can gauge user sentiment and tailor responses in human-computer interaction systems.</t>
+  </si>
+  <si>
+    <t>As a network support specialist, I want to deploy speech to text technology in customer support calls to automatically transcribe user issues and requests related to network connectivity problems, improving response times and issue resolution.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to integrate speech-to-text capabilities into image captioning systems, so that users can verbally describe images and receive accurate textual descriptions generated by the system.</t>
+  </si>
+  <si>
+    <t>As a network security analyst, I want to implement text categorization to automatically classify security alerts and incident reports based on severity levels and types of threats detected, enabling prioritized response and mitigation actions.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to integrate text categorization techniques into medical imaging reports, so that radiological images can be automatically categorized based on clinical findings and diagnoses mentioned in textual reports.</t>
+  </si>
+  <si>
+    <t>As a network troubleshooting expert, I want to deploy unsupervised clustering models to categorize network logs and error reports into clusters based on similar patterns of network issues, facilitating systematic troubleshooting and root cause analysis.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to develop an unsupervised clustering method for organizing and categorizing historical image archives based on visual similarities and metadata, so that cultural heritage collections can be curated and accessed more effectively.</t>
+  </si>
+  <si>
+    <t>As a network support specialist, I want to implement voice recognition technology in customer support calls to automatically transcribe user inquiries and issues related to network connectivity problems, improving service efficiency.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to implement voice recognition in healthcare applications to enable voice-controlled annotation and retrieval of medical images, facilitating efficient diagnosis and treatment planning.</t>
+  </si>
+  <si>
+    <t>As a network performance analyst, I want to implement word embedding models to capture semantic similarities between network performance metrics (e.g., latency, bandwidth) across different network segments, aiding in performance optimization strategies.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to explore word embedding techniques for enhancing the accuracy of image captioning models, enabling more natural and contextually relevant descriptions of visual scenes based on extracted visual features.</t>
   </si>
 </sst>
 </file>
@@ -2226,7 +2355,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2287,6 +2416,12 @@
         <bgColor rgb="FFA2C4C9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE06666"/>
+        <bgColor rgb="FFE06666"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -2316,7 +2451,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2360,6 +2495,7 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2695,10 +2831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F641"/>
+  <dimension ref="A1:F681"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A621" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F621" sqref="F621:F641"/>
+    <sheetView tabSelected="1" topLeftCell="A629" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C643" sqref="C643"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -15530,6 +15666,806 @@
         <v>49</v>
       </c>
     </row>
+    <row r="642" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A642" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B642" s="23">
+        <v>9</v>
+      </c>
+      <c r="C642" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D642" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E642" t="s">
+        <v>708</v>
+      </c>
+      <c r="F642" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="643" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A643" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B643" s="23">
+        <v>9</v>
+      </c>
+      <c r="C643" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D643" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E643" t="s">
+        <v>710</v>
+      </c>
+      <c r="F643" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="644" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A644" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B644" s="23">
+        <v>9</v>
+      </c>
+      <c r="C644" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D644" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E644" t="s">
+        <v>711</v>
+      </c>
+      <c r="F644" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="645" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A645" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B645" s="23">
+        <v>9</v>
+      </c>
+      <c r="C645" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D645" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E645" t="s">
+        <v>712</v>
+      </c>
+      <c r="F645" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="646" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A646" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B646" s="23">
+        <v>9</v>
+      </c>
+      <c r="C646" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D646" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E646" t="s">
+        <v>713</v>
+      </c>
+      <c r="F646" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="647" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A647" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B647" s="23">
+        <v>9</v>
+      </c>
+      <c r="C647" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D647" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E647" t="s">
+        <v>714</v>
+      </c>
+      <c r="F647" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="648" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A648" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B648" s="23">
+        <v>9</v>
+      </c>
+      <c r="C648" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D648" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E648" t="s">
+        <v>715</v>
+      </c>
+      <c r="F648" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="649" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A649" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B649" s="23">
+        <v>9</v>
+      </c>
+      <c r="C649" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D649" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E649" t="s">
+        <v>716</v>
+      </c>
+      <c r="F649" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="650" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A650" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B650" s="23">
+        <v>9</v>
+      </c>
+      <c r="C650" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D650" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E650" t="s">
+        <v>717</v>
+      </c>
+      <c r="F650" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="651" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A651" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B651" s="23">
+        <v>9</v>
+      </c>
+      <c r="C651" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D651" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E651" t="s">
+        <v>718</v>
+      </c>
+      <c r="F651" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="652" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A652" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B652" s="23">
+        <v>9</v>
+      </c>
+      <c r="C652" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D652" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E652" t="s">
+        <v>719</v>
+      </c>
+      <c r="F652" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="653" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A653" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B653" s="23">
+        <v>9</v>
+      </c>
+      <c r="C653" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D653" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E653" t="s">
+        <v>720</v>
+      </c>
+      <c r="F653" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="654" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A654" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B654" s="23">
+        <v>9</v>
+      </c>
+      <c r="C654" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D654" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E654" t="s">
+        <v>721</v>
+      </c>
+      <c r="F654" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="655" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A655" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B655" s="23">
+        <v>9</v>
+      </c>
+      <c r="C655" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D655" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E655" t="s">
+        <v>722</v>
+      </c>
+      <c r="F655" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="656" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A656" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B656" s="23">
+        <v>9</v>
+      </c>
+      <c r="C656" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D656" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E656" t="s">
+        <v>723</v>
+      </c>
+      <c r="F656" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="657" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A657" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B657" s="23">
+        <v>9</v>
+      </c>
+      <c r="C657" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D657" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E657" t="s">
+        <v>724</v>
+      </c>
+      <c r="F657" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="658" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A658" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B658" s="23">
+        <v>9</v>
+      </c>
+      <c r="C658" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D658" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E658" t="s">
+        <v>725</v>
+      </c>
+      <c r="F658" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="659" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A659" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B659" s="23">
+        <v>9</v>
+      </c>
+      <c r="C659" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D659" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E659" t="s">
+        <v>726</v>
+      </c>
+      <c r="F659" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="660" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A660" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B660" s="23">
+        <v>9</v>
+      </c>
+      <c r="C660" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D660" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E660" t="s">
+        <v>727</v>
+      </c>
+      <c r="F660" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="661" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A661" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B661" s="23">
+        <v>9</v>
+      </c>
+      <c r="C661" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D661" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E661" t="s">
+        <v>728</v>
+      </c>
+      <c r="F661" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="662" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A662" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B662" s="23">
+        <v>9</v>
+      </c>
+      <c r="C662" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D662" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E662" t="s">
+        <v>729</v>
+      </c>
+      <c r="F662" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="663" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A663" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B663" s="23">
+        <v>9</v>
+      </c>
+      <c r="C663" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D663" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E663" t="s">
+        <v>730</v>
+      </c>
+      <c r="F663" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="664" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A664" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B664" s="23">
+        <v>9</v>
+      </c>
+      <c r="C664" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D664" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E664" t="s">
+        <v>731</v>
+      </c>
+      <c r="F664" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="665" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A665" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B665" s="23">
+        <v>9</v>
+      </c>
+      <c r="C665" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D665" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E665" t="s">
+        <v>732</v>
+      </c>
+      <c r="F665" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="666" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A666" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B666" s="23">
+        <v>9</v>
+      </c>
+      <c r="C666" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D666" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E666" t="s">
+        <v>733</v>
+      </c>
+      <c r="F666" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="667" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A667" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B667" s="23">
+        <v>9</v>
+      </c>
+      <c r="C667" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D667" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E667" t="s">
+        <v>734</v>
+      </c>
+      <c r="F667" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="668" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A668" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B668" s="23">
+        <v>9</v>
+      </c>
+      <c r="C668" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D668" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E668" t="s">
+        <v>735</v>
+      </c>
+      <c r="F668" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="669" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A669" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B669" s="23">
+        <v>9</v>
+      </c>
+      <c r="C669" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D669" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E669" t="s">
+        <v>736</v>
+      </c>
+      <c r="F669" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="670" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A670" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B670" s="23">
+        <v>9</v>
+      </c>
+      <c r="C670" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D670" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E670" t="s">
+        <v>737</v>
+      </c>
+      <c r="F670" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="671" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A671" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B671" s="23">
+        <v>9</v>
+      </c>
+      <c r="C671" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D671" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E671" t="s">
+        <v>738</v>
+      </c>
+      <c r="F671" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="672" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A672" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B672" s="23">
+        <v>9</v>
+      </c>
+      <c r="C672" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D672" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E672" t="s">
+        <v>739</v>
+      </c>
+      <c r="F672" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="673" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A673" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B673" s="23">
+        <v>9</v>
+      </c>
+      <c r="C673" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D673" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E673" t="s">
+        <v>740</v>
+      </c>
+      <c r="F673" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="674" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A674" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B674" s="23">
+        <v>9</v>
+      </c>
+      <c r="C674" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D674" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E674" t="s">
+        <v>741</v>
+      </c>
+      <c r="F674" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="675" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A675" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B675" s="23">
+        <v>9</v>
+      </c>
+      <c r="C675" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D675" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E675" t="s">
+        <v>742</v>
+      </c>
+      <c r="F675" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="676" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A676" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B676" s="23">
+        <v>9</v>
+      </c>
+      <c r="C676" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D676" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E676" t="s">
+        <v>743</v>
+      </c>
+      <c r="F676" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="677" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A677" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B677" s="23">
+        <v>9</v>
+      </c>
+      <c r="C677" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D677" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E677" t="s">
+        <v>744</v>
+      </c>
+      <c r="F677" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="678" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A678" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B678" s="23">
+        <v>9</v>
+      </c>
+      <c r="C678" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D678" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E678" t="s">
+        <v>745</v>
+      </c>
+      <c r="F678" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="679" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A679" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B679" s="23">
+        <v>9</v>
+      </c>
+      <c r="C679" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D679" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E679" t="s">
+        <v>746</v>
+      </c>
+      <c r="F679" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="680" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A680" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B680" s="23">
+        <v>9</v>
+      </c>
+      <c r="C680" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="D680" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E680" t="s">
+        <v>747</v>
+      </c>
+      <c r="F680" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="681" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A681" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B681" s="23">
+        <v>9</v>
+      </c>
+      <c r="C681" s="23" t="s">
+        <v>709</v>
+      </c>
+      <c r="D681" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E681" t="s">
+        <v>748</v>
+      </c>
+      <c r="F681" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A162:F221">
     <sortCondition ref="D1:D221"/>

</xml_diff>